<commit_message>
Update de ejemplo SW
</commit_message>
<xml_diff>
--- a/Validacion/SW-T2-S3-4/Documentation/Documentacion SW-T2-S3-4.xlsx
+++ b/Validacion/SW-T2-S3-4/Documentation/Documentacion SW-T2-S3-4.xlsx
@@ -42,30 +42,6 @@
     <author>Maria Jose Nuñez</author>
   </authors>
   <commentList>
-    <comment ref="S36" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Maria Jose Nuñez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-ecu = ec-f'c/Ec+2*(Gfc/Lelem)/f'c</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="F37" authorId="0" shapeId="0">
       <text>
         <r>
@@ -90,12 +66,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="S38" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Maria Jose Nuñez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ecu = ec-f'c/Ec+2*(Gfc/Lelem)/f'c</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="91">
   <si>
     <t>X coord [mm]</t>
   </si>
@@ -337,9 +337,6 @@
     <t>Tension softening stiffness</t>
   </si>
   <si>
-    <t>Et</t>
-  </si>
-  <si>
     <t>Ratio between unloading slope at epscu and initial slope</t>
   </si>
   <si>
@@ -362,6 +359,15 @@
   </si>
   <si>
     <t>Lelem</t>
+  </si>
+  <si>
+    <t>strainAtFc_conf</t>
+  </si>
+  <si>
+    <t>E0_conf =  2*Fc/strainAtFc_conf</t>
+  </si>
+  <si>
+    <t>Et = 0,05*E0</t>
   </si>
 </sst>
 </file>
@@ -371,9 +377,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,6 +439,12 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -752,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -801,9 +813,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -901,43 +910,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -959,16 +935,61 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1340,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:U72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T36" sqref="T36"/>
+    <sheetView tabSelected="1" topLeftCell="M27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S42" sqref="S42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,7 +1381,7 @@
     <col min="15" max="15" width="12.28515625" style="1" customWidth="1"/>
     <col min="16" max="17" width="11.42578125" style="1"/>
     <col min="18" max="18" width="48.7109375" style="16" customWidth="1"/>
-    <col min="19" max="19" width="26.42578125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="31.5703125" style="1" customWidth="1"/>
     <col min="20" max="20" width="18.140625" style="1" customWidth="1"/>
     <col min="21" max="21" width="15.85546875" style="1" customWidth="1"/>
     <col min="22" max="22" width="11.42578125" style="1"/>
@@ -1373,13 +1394,13 @@
   <sheetData>
     <row r="7" spans="11:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="11:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K8" s="52" t="s">
+      <c r="K8" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="53"/>
-      <c r="M8" s="53"/>
-      <c r="N8" s="53"/>
-      <c r="O8" s="54"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="69"/>
+      <c r="N8" s="69"/>
+      <c r="O8" s="70"/>
     </row>
     <row r="9" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K9" s="2" t="s">
@@ -1416,14 +1437,14 @@
         <f>N10/10</f>
         <v>0</v>
       </c>
-      <c r="R10" s="65" t="s">
+      <c r="R10" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="S10" s="18" t="s">
+      <c r="S10" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="T10" s="18"/>
-      <c r="U10" s="49"/>
+      <c r="T10" s="17"/>
+      <c r="U10" s="48"/>
     </row>
     <row r="11" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K11" s="4">
@@ -1443,16 +1464,16 @@
         <f t="shared" ref="O11:O33" si="1">N11/10</f>
         <v>0</v>
       </c>
-      <c r="R11" s="66" t="s">
+      <c r="R11" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="S11" s="67" t="s">
+      <c r="S11" s="55" t="s">
         <v>12</v>
       </c>
       <c r="T11" s="13">
         <v>584</v>
       </c>
-      <c r="U11" s="50" t="s">
+      <c r="U11" s="49" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1474,13 +1495,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R12" s="66"/>
-      <c r="S12" s="67"/>
+      <c r="R12" s="54"/>
+      <c r="S12" s="55"/>
       <c r="T12" s="13">
         <f>T11*10.2</f>
         <v>5956.7999999999993</v>
       </c>
-      <c r="U12" s="50" t="s">
+      <c r="U12" s="49" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1502,14 +1523,14 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="R13" s="66"/>
-      <c r="S13" s="67" t="s">
+      <c r="R13" s="54"/>
+      <c r="S13" s="55" t="s">
         <v>13</v>
       </c>
       <c r="T13" s="13">
         <v>584</v>
       </c>
-      <c r="U13" s="50" t="s">
+      <c r="U13" s="49" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1531,13 +1552,13 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="R14" s="66"/>
-      <c r="S14" s="67"/>
+      <c r="R14" s="54"/>
+      <c r="S14" s="55"/>
       <c r="T14" s="13">
         <f>T13*10.2</f>
         <v>5956.7999999999993</v>
       </c>
-      <c r="U14" s="50" t="s">
+      <c r="U14" s="49" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1559,14 +1580,14 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="R15" s="66"/>
-      <c r="S15" s="67" t="s">
+      <c r="R15" s="54"/>
+      <c r="S15" s="55" t="s">
         <v>16</v>
       </c>
       <c r="T15" s="13">
         <v>584</v>
       </c>
-      <c r="U15" s="50" t="s">
+      <c r="U15" s="49" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1588,13 +1609,13 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="R16" s="66"/>
-      <c r="S16" s="67"/>
+      <c r="R16" s="54"/>
+      <c r="S16" s="55"/>
       <c r="T16" s="13">
         <f>T15*10.2</f>
         <v>5956.7999999999993</v>
       </c>
-      <c r="U16" s="50" t="s">
+      <c r="U16" s="49" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1616,14 +1637,14 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="R17" s="66"/>
-      <c r="S17" s="67" t="s">
+      <c r="R17" s="54"/>
+      <c r="S17" s="55" t="s">
         <v>17</v>
       </c>
       <c r="T17" s="13">
         <v>473</v>
       </c>
-      <c r="U17" s="50" t="s">
+      <c r="U17" s="49" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1645,13 +1666,13 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="R18" s="66"/>
-      <c r="S18" s="67"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="55"/>
       <c r="T18" s="13">
         <f>T17*10.2</f>
         <v>4824.5999999999995</v>
       </c>
-      <c r="U18" s="50" t="s">
+      <c r="U18" s="49" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1673,16 +1694,16 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="R19" s="66" t="s">
+      <c r="R19" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="S19" s="67" t="s">
+      <c r="S19" s="55" t="s">
         <v>19</v>
       </c>
       <c r="T19" s="13">
         <v>200000</v>
       </c>
-      <c r="U19" s="50" t="s">
+      <c r="U19" s="49" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1704,13 +1725,13 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="R20" s="66"/>
-      <c r="S20" s="67"/>
+      <c r="R20" s="54"/>
+      <c r="S20" s="55"/>
       <c r="T20" s="13">
         <f>T19*10.2</f>
         <v>2039999.9999999998</v>
       </c>
-      <c r="U20" s="50" t="s">
+      <c r="U20" s="49" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1732,16 +1753,16 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="R21" s="66" t="s">
+      <c r="R21" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="S21" s="67" t="s">
+      <c r="S21" s="55" t="s">
         <v>21</v>
       </c>
       <c r="T21" s="13">
         <v>0</v>
       </c>
-      <c r="U21" s="50"/>
+      <c r="U21" s="49"/>
     </row>
     <row r="22" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K22" s="4">
@@ -1761,16 +1782,16 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="R22" s="68" t="s">
+      <c r="R22" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="S22" s="67" t="s">
+      <c r="S22" s="55" t="s">
         <v>24</v>
       </c>
       <c r="T22" s="13">
         <v>18</v>
       </c>
-      <c r="U22" s="50"/>
+      <c r="U22" s="49"/>
     </row>
     <row r="23" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K23" s="4">
@@ -1790,16 +1811,16 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="R23" s="68" t="s">
+      <c r="R23" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="S23" s="67" t="s">
+      <c r="S23" s="55" t="s">
         <v>25</v>
       </c>
       <c r="T23" s="13">
         <v>0.9</v>
       </c>
-      <c r="U23" s="50"/>
+      <c r="U23" s="49"/>
     </row>
     <row r="24" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K24" s="4">
@@ -1819,14 +1840,14 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="R24" s="66"/>
-      <c r="S24" s="67" t="s">
+      <c r="R24" s="54"/>
+      <c r="S24" s="55" t="s">
         <v>26</v>
       </c>
       <c r="T24" s="13">
         <v>0.15</v>
       </c>
-      <c r="U24" s="50"/>
+      <c r="U24" s="49"/>
     </row>
     <row r="25" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K25" s="4">
@@ -1846,14 +1867,14 @@
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="R25" s="66"/>
-      <c r="S25" s="67" t="s">
+      <c r="R25" s="54"/>
+      <c r="S25" s="55" t="s">
         <v>27</v>
       </c>
       <c r="T25" s="13">
         <v>0</v>
       </c>
-      <c r="U25" s="50"/>
+      <c r="U25" s="49"/>
     </row>
     <row r="26" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K26" s="4">
@@ -1873,14 +1894,14 @@
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="R26" s="66"/>
-      <c r="S26" s="67" t="s">
+      <c r="R26" s="54"/>
+      <c r="S26" s="55" t="s">
         <v>28</v>
       </c>
       <c r="T26" s="13">
         <v>1</v>
       </c>
-      <c r="U26" s="50"/>
+      <c r="U26" s="49"/>
     </row>
     <row r="27" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K27" s="4">
@@ -1900,14 +1921,14 @@
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="R27" s="66"/>
-      <c r="S27" s="67" t="s">
+      <c r="R27" s="54"/>
+      <c r="S27" s="55" t="s">
         <v>29</v>
       </c>
       <c r="T27" s="13">
         <v>0</v>
       </c>
-      <c r="U27" s="50"/>
+      <c r="U27" s="49"/>
     </row>
     <row r="28" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K28" s="4">
@@ -1927,14 +1948,14 @@
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-      <c r="R28" s="69"/>
-      <c r="S28" s="42" t="s">
+      <c r="R28" s="57"/>
+      <c r="S28" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="T28" s="70">
+      <c r="T28" s="58">
         <v>1</v>
       </c>
-      <c r="U28" s="71"/>
+      <c r="U28" s="59"/>
     </row>
     <row r="29" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K29" s="4">
@@ -1954,12 +1975,14 @@
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-      <c r="R29" s="16" t="s">
+      <c r="R29" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="S29" s="17" t="s">
+      <c r="S29" s="73" t="s">
         <v>63</v>
       </c>
+      <c r="T29" s="17"/>
+      <c r="U29" s="51"/>
     </row>
     <row r="30" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K30" s="4">
@@ -1979,16 +2002,16 @@
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-      <c r="R30" s="16" t="s">
+      <c r="R30" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="S30" s="1" t="s">
+      <c r="S30" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="T30" s="72">
+      <c r="T30" s="74">
         <v>-29</v>
       </c>
-      <c r="U30" s="1" t="s">
+      <c r="U30" s="52" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2010,15 +2033,16 @@
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
-      <c r="R31" s="16" t="s">
+      <c r="R31" s="54" t="s">
         <v>66</v>
       </c>
-      <c r="S31" s="1" t="s">
+      <c r="S31" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="T31" s="73">
+      <c r="T31" s="75">
         <v>-2E-3</v>
       </c>
+      <c r="U31" s="52"/>
     </row>
     <row r="32" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K32" s="4">
@@ -2038,18 +2062,11 @@
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
-      <c r="R32" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="S32" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="T32" s="1">
-        <f>2*T30/T31</f>
-        <v>29000</v>
-      </c>
-      <c r="U32" s="1" t="s">
-        <v>70</v>
+      <c r="S32" s="78" t="s">
+        <v>88</v>
+      </c>
+      <c r="T32" s="78">
+        <v>-5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2070,113 +2087,114 @@
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
-      <c r="R33" s="16" t="s">
+      <c r="R33" s="54" t="s">
+        <v>68</v>
+      </c>
+      <c r="S33" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="T33" s="13">
+        <f>2*T30/T31</f>
+        <v>29000</v>
+      </c>
+      <c r="U33" s="52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S34" s="78" t="s">
+        <v>89</v>
+      </c>
+      <c r="T34" s="78">
+        <f>2*T30/T32</f>
+        <v>11600</v>
+      </c>
+      <c r="U34" s="78" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" s="38">
+        <v>750</v>
+      </c>
+      <c r="F35" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="K35" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="L35" s="69"/>
+      <c r="M35" s="69"/>
+      <c r="N35" s="69"/>
+      <c r="O35" s="70"/>
+      <c r="R35" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="S33" s="1" t="s">
+      <c r="S35" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="T33" s="1">
-        <v>0</v>
-      </c>
-      <c r="U33" s="1" t="s">
+      <c r="T35" s="13">
+        <v>0</v>
+      </c>
+      <c r="U35" s="52" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R34" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="S34" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="T34" s="1">
-        <f>Hoja1!F9</f>
-        <v>240</v>
-      </c>
-      <c r="U34" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="D35" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="E35" s="39">
-        <v>750</v>
-      </c>
-      <c r="F35" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="K35" s="52" t="s">
-        <v>5</v>
-      </c>
-      <c r="L35" s="53"/>
-      <c r="M35" s="53"/>
-      <c r="N35" s="53"/>
-      <c r="O35" s="54"/>
-      <c r="R35" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="S35" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="T35" s="1">
-        <v>87.6</v>
-      </c>
-      <c r="U35" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C36" s="38" t="s">
+      <c r="C36" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="D36" s="45" t="s">
+      <c r="D36" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="E36" s="39">
+      <c r="E36" s="38">
         <f>L33</f>
         <v>1500</v>
       </c>
-      <c r="F36" s="21" t="s">
+      <c r="F36" s="20" t="s">
         <v>53</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L36" s="55" t="s">
+      <c r="L36" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="M36" s="55"/>
-      <c r="N36" s="55"/>
-      <c r="O36" s="56"/>
-      <c r="R36" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="S36" s="1" t="s">
+      <c r="M36" s="71"/>
+      <c r="N36" s="71"/>
+      <c r="O36" s="72"/>
+      <c r="R36" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="S36" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="T36" s="74">
-        <f>T31-T30/T32+2*(T35/T34)/T30</f>
-        <v>-2.617241379310345E-2</v>
+      <c r="T36" s="13">
+        <f>N13</f>
+        <v>150</v>
+      </c>
+      <c r="U36" s="52" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="D37" s="42" t="s">
+      <c r="D37" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="E37" s="43">
+      <c r="E37" s="42">
         <f>E35/E36</f>
         <v>0.5</v>
       </c>
-      <c r="F37" s="44" t="s">
+      <c r="F37" s="43" t="s">
         <v>58</v>
       </c>
       <c r="K37" s="4">
@@ -2194,18 +2212,17 @@
       <c r="O37" s="14">
         <v>4</v>
       </c>
-      <c r="R37" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="S37" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="T37" s="75">
-        <f>0.31*ABS(T30)^(1/2)</f>
-        <v>1.6694010902116962</v>
-      </c>
-      <c r="U37" s="1" t="s">
-        <v>15</v>
+      <c r="R37" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="S37" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="T37" s="13">
+        <v>87.6</v>
+      </c>
+      <c r="U37" s="52" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -2224,15 +2241,17 @@
       <c r="O38" s="14">
         <v>5</v>
       </c>
-      <c r="R38" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="S38" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="T38" s="1">
-        <v>8.0000000000000007E-5</v>
-      </c>
+      <c r="R38" s="54" t="s">
+        <v>74</v>
+      </c>
+      <c r="S38" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="T38" s="76">
+        <f>T31-T30/T33+2*(T37/T36)/T30</f>
+        <v>-4.1275862068965517E-2</v>
+      </c>
+      <c r="U38" s="52"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K39" s="4">
@@ -2250,18 +2269,18 @@
       <c r="O39" s="14">
         <v>7</v>
       </c>
-      <c r="R39" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="S39" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="T39" s="1">
-        <f>0.05*T32</f>
-        <v>1450</v>
-      </c>
-      <c r="U39" s="1" t="s">
-        <v>73</v>
+      <c r="R39" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="S39" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="T39" s="77">
+        <f>0.31*ABS(T30)^(1/2)</f>
+        <v>1.6694010902116962</v>
+      </c>
+      <c r="U39" s="52" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
@@ -2280,15 +2299,16 @@
       <c r="O40" s="14">
         <v>8</v>
       </c>
-      <c r="R40" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="S40" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="T40" s="1">
-        <v>0.1</v>
-      </c>
+      <c r="R40" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="S40" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="T40" s="13">
+        <v>8.0000000000000007E-5</v>
+      </c>
+      <c r="U40" s="52"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K41" s="4">
@@ -2306,6 +2326,19 @@
       <c r="O41" s="14">
         <v>10</v>
       </c>
+      <c r="R41" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="S41" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="T41" s="13">
+        <f>0.05*T33</f>
+        <v>1450</v>
+      </c>
+      <c r="U41" s="52" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K42" s="4">
@@ -2323,21 +2356,31 @@
       <c r="O42" s="14">
         <v>11</v>
       </c>
+      <c r="R42" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="S42" s="58" t="s">
+        <v>81</v>
+      </c>
+      <c r="T42" s="58">
+        <v>0.1</v>
+      </c>
+      <c r="U42" s="59"/>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
-      <c r="D43" s="57" t="s">
+      <c r="D43" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="E43" s="58"/>
-      <c r="F43" s="26" t="s">
+      <c r="E43" s="63"/>
+      <c r="F43" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G43" s="57" t="s">
+      <c r="G43" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="H43" s="58"/>
-      <c r="I43" s="26" t="s">
+      <c r="H43" s="63"/>
+      <c r="I43" s="25" t="s">
         <v>37</v>
       </c>
       <c r="K43" s="4">
@@ -2358,18 +2401,18 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
-      <c r="D44" s="59" t="s">
+      <c r="D44" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="E44" s="60"/>
-      <c r="F44" s="27" t="s">
+      <c r="E44" s="65"/>
+      <c r="F44" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="G44" s="59" t="s">
+      <c r="G44" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="H44" s="60"/>
-      <c r="I44" s="27" t="s">
+      <c r="H44" s="65"/>
+      <c r="I44" s="26" t="s">
         <v>49</v>
       </c>
       <c r="K44" s="4">
@@ -2393,22 +2436,22 @@
       <c r="C45" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D45" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E45" s="23" t="s">
+      <c r="E45" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="F45" s="27" t="s">
+      <c r="F45" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="G45" s="22" t="s">
+      <c r="G45" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="I45" s="27" t="s">
+      <c r="I45" s="26" t="s">
         <v>48</v>
       </c>
       <c r="K45" s="4">
@@ -2428,19 +2471,19 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="63" t="s">
+      <c r="A46" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="64"/>
-      <c r="C46" s="20">
+      <c r="B46" s="67"/>
+      <c r="C46" s="19">
         <v>1</v>
       </c>
-      <c r="D46" s="24"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="28"/>
+      <c r="D46" s="23"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="27"/>
       <c r="K46" s="4">
         <v>10</v>
       </c>
@@ -2458,29 +2501,29 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="61" t="s">
+      <c r="A47" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="18"/>
-      <c r="D47" s="25">
+      <c r="C47" s="17"/>
+      <c r="D47" s="24">
         <v>2</v>
       </c>
-      <c r="E47" s="19">
+      <c r="E47" s="18">
         <v>3</v>
       </c>
-      <c r="F47" s="26">
+      <c r="F47" s="25">
         <v>10</v>
       </c>
-      <c r="G47" s="25">
+      <c r="G47" s="24">
         <v>20</v>
       </c>
-      <c r="H47" s="19">
+      <c r="H47" s="18">
         <v>21</v>
       </c>
-      <c r="I47" s="26">
+      <c r="I47" s="25">
         <v>30</v>
       </c>
       <c r="K47" s="4">
@@ -2500,27 +2543,27 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="62"/>
-      <c r="B48" s="29" t="s">
+      <c r="A48" s="61"/>
+      <c r="B48" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C48" s="29"/>
-      <c r="D48" s="30">
+      <c r="C48" s="28"/>
+      <c r="D48" s="29">
         <v>4</v>
       </c>
-      <c r="E48" s="31">
+      <c r="E48" s="30">
         <v>5</v>
       </c>
-      <c r="F48" s="32">
+      <c r="F48" s="31">
         <v>11</v>
       </c>
-      <c r="G48" s="30">
+      <c r="G48" s="29">
         <v>22</v>
       </c>
-      <c r="H48" s="31">
+      <c r="H48" s="30">
         <v>23</v>
       </c>
-      <c r="I48" s="32">
+      <c r="I48" s="31">
         <v>31</v>
       </c>
       <c r="K48" s="4">
@@ -2540,29 +2583,29 @@
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="61" t="s">
+      <c r="A49" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="B49" s="33" t="s">
+      <c r="B49" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C49" s="33"/>
-      <c r="D49" s="34">
+      <c r="C49" s="32"/>
+      <c r="D49" s="33">
         <v>6</v>
       </c>
-      <c r="E49" s="35">
+      <c r="E49" s="34">
         <v>7</v>
       </c>
-      <c r="F49" s="36">
+      <c r="F49" s="35">
         <v>12</v>
       </c>
-      <c r="G49" s="34">
+      <c r="G49" s="33">
         <v>24</v>
       </c>
-      <c r="H49" s="35">
+      <c r="H49" s="34">
         <v>25</v>
       </c>
-      <c r="I49" s="36">
+      <c r="I49" s="35">
         <v>32</v>
       </c>
       <c r="K49" s="4">
@@ -2582,27 +2625,27 @@
       </c>
     </row>
     <row r="50" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="62"/>
-      <c r="B50" s="29" t="s">
+      <c r="A50" s="61"/>
+      <c r="B50" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="30">
+      <c r="C50" s="28"/>
+      <c r="D50" s="29">
         <v>8</v>
       </c>
-      <c r="E50" s="31">
+      <c r="E50" s="30">
         <v>9</v>
       </c>
-      <c r="F50" s="32">
+      <c r="F50" s="31">
         <v>13</v>
       </c>
-      <c r="G50" s="30">
+      <c r="G50" s="29">
         <v>26</v>
       </c>
-      <c r="H50" s="31">
+      <c r="H50" s="30">
         <v>27</v>
       </c>
-      <c r="I50" s="32">
+      <c r="I50" s="31">
         <v>33</v>
       </c>
       <c r="K50" s="5">
@@ -2783,16 +2826,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="K8:O8"/>
+    <mergeCell ref="L36:O36"/>
+    <mergeCell ref="K35:O35"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="G43:H43"/>
     <mergeCell ref="G44:H44"/>
     <mergeCell ref="A46:B46"/>
-    <mergeCell ref="K8:O8"/>
-    <mergeCell ref="L36:O36"/>
-    <mergeCell ref="K35:O35"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2811,35 +2854,35 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="46"/>
-    <col min="3" max="3" width="10.85546875" style="46" customWidth="1"/>
-    <col min="4" max="4" width="22" style="46" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="46" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="46" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="46"/>
+    <col min="1" max="2" width="11.42578125" style="45"/>
+    <col min="3" max="3" width="10.85546875" style="45" customWidth="1"/>
+    <col min="4" max="4" width="22" style="45" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" style="45" customWidth="1"/>
+    <col min="6" max="6" width="25.85546875" style="45" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="45"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="54"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="70"/>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="39" t="s">
         <v>2</v>
       </c>
       <c r="G5" s="10" t="s">
@@ -2853,7 +2896,7 @@
       <c r="D6" s="13">
         <v>0</v>
       </c>
-      <c r="E6" s="51">
+      <c r="E6" s="50">
         <f>D6/10</f>
         <v>0</v>
       </c>
@@ -2872,7 +2915,7 @@
       <c r="D7" s="13">
         <v>750</v>
       </c>
-      <c r="E7" s="51">
+      <c r="E7" s="50">
         <f t="shared" ref="E7:E29" si="0">D7/10</f>
         <v>75</v>
       </c>
@@ -2891,7 +2934,7 @@
       <c r="D8" s="13">
         <v>1500</v>
       </c>
-      <c r="E8" s="51">
+      <c r="E8" s="50">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
@@ -2910,7 +2953,7 @@
       <c r="D9" s="13">
         <v>0</v>
       </c>
-      <c r="E9" s="51">
+      <c r="E9" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2929,7 +2972,7 @@
       <c r="D10" s="13">
         <v>750</v>
       </c>
-      <c r="E10" s="51">
+      <c r="E10" s="50">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
@@ -2948,7 +2991,7 @@
       <c r="D11" s="13">
         <v>1500</v>
       </c>
-      <c r="E11" s="51">
+      <c r="E11" s="50">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
@@ -2967,7 +3010,7 @@
       <c r="D12" s="13">
         <v>0</v>
       </c>
-      <c r="E12" s="51">
+      <c r="E12" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2987,7 +3030,7 @@
       <c r="D13" s="13">
         <v>750</v>
       </c>
-      <c r="E13" s="51">
+      <c r="E13" s="50">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
@@ -3007,7 +3050,7 @@
       <c r="D14" s="13">
         <v>1500</v>
       </c>
-      <c r="E14" s="51">
+      <c r="E14" s="50">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
@@ -3027,7 +3070,7 @@
       <c r="D15" s="13">
         <v>0</v>
       </c>
-      <c r="E15" s="51">
+      <c r="E15" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3047,7 +3090,7 @@
       <c r="D16" s="13">
         <v>750</v>
       </c>
-      <c r="E16" s="51">
+      <c r="E16" s="50">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
@@ -3067,7 +3110,7 @@
       <c r="D17" s="13">
         <v>1500</v>
       </c>
-      <c r="E17" s="51">
+      <c r="E17" s="50">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
@@ -3087,7 +3130,7 @@
       <c r="D18" s="13">
         <v>0</v>
       </c>
-      <c r="E18" s="51">
+      <c r="E18" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3107,7 +3150,7 @@
       <c r="D19" s="13">
         <v>750</v>
       </c>
-      <c r="E19" s="51">
+      <c r="E19" s="50">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
@@ -3127,7 +3170,7 @@
       <c r="D20" s="13">
         <v>1500</v>
       </c>
-      <c r="E20" s="51">
+      <c r="E20" s="50">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
@@ -3147,7 +3190,7 @@
       <c r="D21" s="13">
         <v>0</v>
       </c>
-      <c r="E21" s="51">
+      <c r="E21" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3167,7 +3210,7 @@
       <c r="D22" s="13">
         <v>750</v>
       </c>
-      <c r="E22" s="51">
+      <c r="E22" s="50">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
@@ -3187,7 +3230,7 @@
       <c r="D23" s="13">
         <v>1500</v>
       </c>
-      <c r="E23" s="51">
+      <c r="E23" s="50">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
@@ -3207,7 +3250,7 @@
       <c r="D24" s="13">
         <v>0</v>
       </c>
-      <c r="E24" s="51">
+      <c r="E24" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3227,7 +3270,7 @@
       <c r="D25" s="13">
         <v>750</v>
       </c>
-      <c r="E25" s="51">
+      <c r="E25" s="50">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
@@ -3247,7 +3290,7 @@
       <c r="D26" s="13">
         <v>1500</v>
       </c>
-      <c r="E26" s="51">
+      <c r="E26" s="50">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
@@ -3267,7 +3310,7 @@
       <c r="D27" s="13">
         <v>0</v>
       </c>
-      <c r="E27" s="51">
+      <c r="E27" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3287,7 +3330,7 @@
       <c r="D28" s="13">
         <v>750</v>
       </c>
-      <c r="E28" s="51">
+      <c r="E28" s="50">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
@@ -3417,7 +3460,7 @@
       </c>
     </row>
     <row r="3" spans="3:70" x14ac:dyDescent="0.25">
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="36" t="s">
         <v>60</v>
       </c>
       <c r="D3">
@@ -3623,274 +3666,274 @@
       </c>
     </row>
     <row r="4" spans="3:70" x14ac:dyDescent="0.25">
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="47">
+      <c r="D4" s="46">
         <f>(D3/$D$2)*100</f>
         <v>0</v>
       </c>
-      <c r="E4" s="48">
+      <c r="E4" s="47">
         <f>(E3/$D$2)*100</f>
         <v>4.2105263157894736E-2</v>
       </c>
-      <c r="F4" s="48">
+      <c r="F4" s="47">
         <f t="shared" ref="F4:I4" si="0">(F3/$D$2)*100</f>
         <v>-4.2105263157894736E-2</v>
       </c>
-      <c r="G4" s="48">
+      <c r="G4" s="47">
         <f>(G3/$D$2)*100</f>
         <v>8.4210526315789472E-2</v>
       </c>
-      <c r="H4" s="48">
+      <c r="H4" s="47">
         <f t="shared" si="0"/>
         <v>-8.4210526315789472E-2</v>
       </c>
-      <c r="I4" s="48">
+      <c r="I4" s="47">
         <f t="shared" si="0"/>
         <v>0.12631578947368421</v>
       </c>
-      <c r="J4" s="48">
+      <c r="J4" s="47">
         <f t="shared" ref="J4" si="1">(J3/$D$2)*100</f>
         <v>-0.12631578947368421</v>
       </c>
-      <c r="K4" s="48">
+      <c r="K4" s="47">
         <f t="shared" ref="K4" si="2">(K3/$D$2)*100</f>
         <v>0.15789473684210525</v>
       </c>
-      <c r="L4" s="48">
+      <c r="L4" s="47">
         <f t="shared" ref="L4" si="3">(L3/$D$2)*100</f>
         <v>-0.15789473684210525</v>
       </c>
-      <c r="M4" s="48">
+      <c r="M4" s="47">
         <f t="shared" ref="M4:N4" si="4">(M3/$D$2)*100</f>
         <v>0.24210526315789474</v>
       </c>
-      <c r="N4" s="48">
+      <c r="N4" s="47">
         <f t="shared" si="4"/>
         <v>-0.24210526315789474</v>
       </c>
-      <c r="O4" s="48">
+      <c r="O4" s="47">
         <f t="shared" ref="O4" si="5">(O3/$D$2)*100</f>
         <v>0.31578947368421051</v>
       </c>
-      <c r="P4" s="48">
+      <c r="P4" s="47">
         <f t="shared" ref="P4" si="6">(P3/$D$2)*100</f>
         <v>-0.31578947368421051</v>
       </c>
-      <c r="Q4" s="48">
+      <c r="Q4" s="47">
         <f t="shared" ref="Q4" si="7">(Q3/$D$2)*100</f>
         <v>0.47368421052631582</v>
       </c>
-      <c r="R4" s="48">
+      <c r="R4" s="47">
         <f t="shared" ref="R4:S4" si="8">(R3/$D$2)*100</f>
         <v>-0.47368421052631582</v>
       </c>
-      <c r="S4" s="48">
+      <c r="S4" s="47">
         <f t="shared" si="8"/>
         <v>0.47368421052631582</v>
       </c>
-      <c r="T4" s="48">
+      <c r="T4" s="47">
         <f t="shared" ref="T4" si="9">(T3/$D$2)*100</f>
         <v>-0.47368421052631582</v>
       </c>
-      <c r="U4" s="48">
+      <c r="U4" s="47">
         <f t="shared" ref="U4" si="10">(U3/$D$2)*100</f>
         <v>0.47368421052631582</v>
       </c>
-      <c r="V4" s="48">
+      <c r="V4" s="47">
         <f t="shared" ref="V4" si="11">(V3/$D$2)*100</f>
         <v>-0.47368421052631582</v>
       </c>
-      <c r="W4" s="48">
+      <c r="W4" s="47">
         <f t="shared" ref="W4:X4" si="12">(W3/$D$2)*100</f>
         <v>0.63157894736842102</v>
       </c>
-      <c r="X4" s="48">
+      <c r="X4" s="47">
         <f t="shared" si="12"/>
         <v>-0.63157894736842102</v>
       </c>
-      <c r="Y4" s="48">
+      <c r="Y4" s="47">
         <f t="shared" ref="Y4" si="13">(Y3/$D$2)*100</f>
         <v>0.63157894736842102</v>
       </c>
-      <c r="Z4" s="48">
+      <c r="Z4" s="47">
         <f t="shared" ref="Z4" si="14">(Z3/$D$2)*100</f>
         <v>-0.63157894736842102</v>
       </c>
-      <c r="AA4" s="48">
+      <c r="AA4" s="47">
         <f t="shared" ref="AA4" si="15">(AA3/$D$2)*100</f>
         <v>0.63157894736842102</v>
       </c>
-      <c r="AB4" s="48">
+      <c r="AB4" s="47">
         <f t="shared" ref="AB4:AC4" si="16">(AB3/$D$2)*100</f>
         <v>-0.63157894736842102</v>
       </c>
-      <c r="AC4" s="48">
+      <c r="AC4" s="47">
         <f t="shared" si="16"/>
         <v>0.78947368421052633</v>
       </c>
-      <c r="AD4" s="48">
+      <c r="AD4" s="47">
         <f t="shared" ref="AD4" si="17">(AD3/$D$2)*100</f>
         <v>-0.78947368421052633</v>
       </c>
-      <c r="AE4" s="48">
+      <c r="AE4" s="47">
         <f t="shared" ref="AE4" si="18">(AE3/$D$2)*100</f>
         <v>0.78947368421052633</v>
       </c>
-      <c r="AF4" s="48">
+      <c r="AF4" s="47">
         <f t="shared" ref="AF4" si="19">(AF3/$D$2)*100</f>
         <v>-0.78947368421052633</v>
       </c>
-      <c r="AG4" s="48">
+      <c r="AG4" s="47">
         <f t="shared" ref="AG4:AH4" si="20">(AG3/$D$2)*100</f>
         <v>0.78947368421052633</v>
       </c>
-      <c r="AH4" s="48">
+      <c r="AH4" s="47">
         <f t="shared" si="20"/>
         <v>-0.78947368421052633</v>
       </c>
-      <c r="AI4" s="48">
+      <c r="AI4" s="47">
         <f t="shared" ref="AI4" si="21">(AI3/$D$2)*100</f>
         <v>0.94736842105263164</v>
       </c>
-      <c r="AJ4" s="48">
+      <c r="AJ4" s="47">
         <f t="shared" ref="AJ4" si="22">(AJ3/$D$2)*100</f>
         <v>-0.94736842105263164</v>
       </c>
-      <c r="AK4" s="48">
+      <c r="AK4" s="47">
         <f t="shared" ref="AK4" si="23">(AK3/$D$2)*100</f>
         <v>0.94736842105263164</v>
       </c>
-      <c r="AL4" s="48">
+      <c r="AL4" s="47">
         <f t="shared" ref="AL4:AM4" si="24">(AL3/$D$2)*100</f>
         <v>-0.94736842105263164</v>
       </c>
-      <c r="AM4" s="48">
+      <c r="AM4" s="47">
         <f t="shared" si="24"/>
         <v>0.94736842105263164</v>
       </c>
-      <c r="AN4" s="48">
+      <c r="AN4" s="47">
         <f t="shared" ref="AN4" si="25">(AN3/$D$2)*100</f>
         <v>-0.94736842105263164</v>
       </c>
-      <c r="AO4" s="48">
+      <c r="AO4" s="47">
         <f t="shared" ref="AO4" si="26">(AO3/$D$2)*100</f>
         <v>1.1052631578947369</v>
       </c>
-      <c r="AP4" s="48">
+      <c r="AP4" s="47">
         <f t="shared" ref="AP4" si="27">(AP3/$D$2)*100</f>
         <v>-1.1052631578947369</v>
       </c>
-      <c r="AQ4" s="48">
+      <c r="AQ4" s="47">
         <f t="shared" ref="AQ4:AR4" si="28">(AQ3/$D$2)*100</f>
         <v>1.1052631578947369</v>
       </c>
-      <c r="AR4" s="48">
+      <c r="AR4" s="47">
         <f t="shared" si="28"/>
         <v>-1.1052631578947369</v>
       </c>
-      <c r="AS4" s="48">
+      <c r="AS4" s="47">
         <f t="shared" ref="AS4" si="29">(AS3/$D$2)*100</f>
         <v>1.1052631578947369</v>
       </c>
-      <c r="AT4" s="48">
+      <c r="AT4" s="47">
         <f t="shared" ref="AT4" si="30">(AT3/$D$2)*100</f>
         <v>-1.1052631578947369</v>
       </c>
-      <c r="AU4" s="48">
+      <c r="AU4" s="47">
         <f t="shared" ref="AU4" si="31">(AU3/$D$2)*100</f>
         <v>1.263157894736842</v>
       </c>
-      <c r="AV4" s="48">
+      <c r="AV4" s="47">
         <f t="shared" ref="AV4:AW4" si="32">(AV3/$D$2)*100</f>
         <v>-1.263157894736842</v>
       </c>
-      <c r="AW4" s="48">
+      <c r="AW4" s="47">
         <f t="shared" si="32"/>
         <v>1.263157894736842</v>
       </c>
-      <c r="AX4" s="48">
+      <c r="AX4" s="47">
         <f t="shared" ref="AX4" si="33">(AX3/$D$2)*100</f>
         <v>-1.263157894736842</v>
       </c>
-      <c r="AY4" s="48">
+      <c r="AY4" s="47">
         <f t="shared" ref="AY4" si="34">(AY3/$D$2)*100</f>
         <v>1.263157894736842</v>
       </c>
-      <c r="AZ4" s="48">
+      <c r="AZ4" s="47">
         <f t="shared" ref="AZ4" si="35">(AZ3/$D$2)*100</f>
         <v>-1.263157894736842</v>
       </c>
-      <c r="BA4" s="48">
+      <c r="BA4" s="47">
         <f t="shared" ref="BA4:BB4" si="36">(BA3/$D$2)*100</f>
         <v>1.4210526315789473</v>
       </c>
-      <c r="BB4" s="48">
+      <c r="BB4" s="47">
         <f t="shared" si="36"/>
         <v>-1.4210526315789473</v>
       </c>
-      <c r="BC4" s="48">
+      <c r="BC4" s="47">
         <f t="shared" ref="BC4" si="37">(BC3/$D$2)*100</f>
         <v>1.4210526315789473</v>
       </c>
-      <c r="BD4" s="48">
+      <c r="BD4" s="47">
         <f t="shared" ref="BD4" si="38">(BD3/$D$2)*100</f>
         <v>-1.4210526315789473</v>
       </c>
-      <c r="BE4" s="48">
+      <c r="BE4" s="47">
         <f t="shared" ref="BE4" si="39">(BE3/$D$2)*100</f>
         <v>1.4210526315789473</v>
       </c>
-      <c r="BF4" s="48">
+      <c r="BF4" s="47">
         <f t="shared" ref="BF4:BG4" si="40">(BF3/$D$2)*100</f>
         <v>-1.4210526315789473</v>
       </c>
-      <c r="BG4" s="48">
+      <c r="BG4" s="47">
         <f t="shared" si="40"/>
         <v>1.5789473684210527</v>
       </c>
-      <c r="BH4" s="48">
+      <c r="BH4" s="47">
         <f t="shared" ref="BH4" si="41">(BH3/$D$2)*100</f>
         <v>-1.5789473684210527</v>
       </c>
-      <c r="BI4" s="48">
+      <c r="BI4" s="47">
         <f t="shared" ref="BI4" si="42">(BI3/$D$2)*100</f>
         <v>1.5789473684210527</v>
       </c>
-      <c r="BJ4" s="48">
+      <c r="BJ4" s="47">
         <f t="shared" ref="BJ4" si="43">(BJ3/$D$2)*100</f>
         <v>-1.5789473684210527</v>
       </c>
-      <c r="BK4" s="48">
+      <c r="BK4" s="47">
         <f t="shared" ref="BK4:BL4" si="44">(BK3/$D$2)*100</f>
         <v>1.5789473684210527</v>
       </c>
-      <c r="BL4" s="48">
+      <c r="BL4" s="47">
         <f t="shared" si="44"/>
         <v>-1.5789473684210527</v>
       </c>
-      <c r="BM4" s="48">
+      <c r="BM4" s="47">
         <f t="shared" ref="BM4" si="45">(BM3/$D$2)*100</f>
         <v>1.8947368421052633</v>
       </c>
-      <c r="BN4" s="48">
+      <c r="BN4" s="47">
         <f t="shared" ref="BN4" si="46">(BN3/$D$2)*100</f>
         <v>-1.8947368421052633</v>
       </c>
-      <c r="BO4" s="48">
+      <c r="BO4" s="47">
         <f t="shared" ref="BO4" si="47">(BO3/$D$2)*100</f>
         <v>1.8947368421052633</v>
       </c>
-      <c r="BP4" s="48">
+      <c r="BP4" s="47">
         <f t="shared" ref="BP4:BQ4" si="48">(BP3/$D$2)*100</f>
         <v>-1.8947368421052633</v>
       </c>
-      <c r="BQ4" s="48">
+      <c r="BQ4" s="47">
         <f t="shared" si="48"/>
         <v>1.8947368421052633</v>
       </c>
-      <c r="BR4" s="48">
+      <c r="BR4" s="47">
         <f t="shared" ref="BR4" si="49">(BR3/$D$2)*100</f>
         <v>-1.8947368421052633</v>
       </c>

</xml_diff>

<commit_message>
Se agregan nuevos datos
</commit_message>
<xml_diff>
--- a/Validacion/SW-T2-S3-4/Documentation/Documentacion SW-T2-S3-4.xlsx
+++ b/Validacion/SW-T2-S3-4/Documentation/Documentacion SW-T2-S3-4.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="3" r:id="rId2"/>
     <sheet name=" Drift y Factor de daño  " sheetId="2" r:id="rId3"/>
+    <sheet name="Respuesta local experimental" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -95,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="128">
   <si>
     <t>X coord [mm]</t>
   </si>
@@ -467,6 +468,18 @@
   </si>
   <si>
     <t>3 ciclos</t>
+  </si>
+  <si>
+    <t>Height (mm)</t>
+  </si>
+  <si>
+    <t>Drift</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Negative</t>
   </si>
 </sst>
 </file>
@@ -479,7 +492,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.00.E+00"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -546,6 +559,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -878,7 +899,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1184,6 +1205,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1230,6 +1252,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1247,6 +1284,3394 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$C$6:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.0158730158730101E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6428571428571399E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.95238095238095E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4285714285714199E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.65079365079365E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5D22-455C-B1B5-5D1D45ED16AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>0,80%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$D$6:$D$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.9047619047618999E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.84126984126984E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5238095238095199E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1428571428571399E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0634920634920595E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5D22-455C-B1B5-5D1D45ED16AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>0,60%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$E$6:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-2.38095238095242E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0873015873015799E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1587301587301501E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.2063492063492001E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8730158730158598E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5D22-455C-B1B5-5D1D45ED16AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>0,40%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$F$6:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-4.7619047619048E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2698412698412604E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.1746031746031704E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.8253968253968202E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4444444444444398E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5D22-455C-B1B5-5D1D45ED16AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>0,30%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$G$6:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-3.9682539682540001E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9682539682539601E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.7936507936507905E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8412698412698399E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0952380952380901E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-5D22-455C-B1B5-5D1D45ED16AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>0,20%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$H$6:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-3.9682539682540001E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.26984126984126E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0952380952380901E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6190476190476099E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.19047619047618E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-5D22-455C-B1B5-5D1D45ED16AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>0,15%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$I$6:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-2.38095238095242E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.58730158730155E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.74603174603174E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3492063492063399E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-7.9365079365082292E-6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-5D22-455C-B1B5-5D1D45ED16AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>0,10%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$J$6:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-3.9682539682540001E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.38095238095242E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5555555555555402E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9682539682539398E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.7619047619048E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-5D22-455C-B1B5-5D1D45ED16AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>0,05%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$K$6:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-3.9682539682540001E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3.1746031746032199E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.1746031746032199E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.1746031746032199E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.9682539682540001E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-5D22-455C-B1B5-5D1D45ED16AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1487598416"/>
+        <c:axId val="1487595088"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1487598416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5.000000000000001E-3"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CL"/>
+                  <a:t>Horizontal</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-CL" baseline="0"/>
+                  <a:t> Strain</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-CL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1487595088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1487595088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CL"/>
+                  <a:t>Height</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-CL" baseline="0"/>
+                  <a:t> (mm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-CL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1487598416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.70634747269494536"/>
+          <c:y val="0.25954615048118984"/>
+          <c:w val="0.23263116304010387"/>
+          <c:h val="0.49942621755613881"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$L$6:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.47976197266107E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2906138899979E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8004905036217401E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3450065590600499E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4043042643396203E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-74F4-4649-AF8E-F0EEE6EA8986}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>0,80%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$M$6:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8.4309587634745899E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6955075191543499E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.440673777068E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0820357801479101E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5046673891138596E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-74F4-4649-AF8E-F0EEE6EA8986}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>0,60%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$N$6:$N$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.4175744786022501E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1141656685488301E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.06002015247438E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.9138386661343303E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.3282191676647801E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-74F4-4649-AF8E-F0EEE6EA8986}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>0,40%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$O$6:$O$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.6540428525256898E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.05180706857544E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.72522291298313E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.4917393866803503E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4285822924390102E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-74F4-4649-AF8E-F0EEE6EA8986}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>0,30%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$P$6:$P$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.7795775585084703E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.25253331812391E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8567463259757698E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1076826555637902E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.4597425806574199E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-74F4-4649-AF8E-F0EEE6EA8986}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>0,20%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$Q$6:$Q$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.7415540219392903E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.31485389456073E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.78028099393524E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.37761174166809E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.21371128728682E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-74F4-4649-AF8E-F0EEE6EA8986}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>0,15%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$R$6:$R$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.7415540219392903E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4601418277913698E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5346299359303301E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.13196068366318E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.45251810870926E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-74F4-4649-AF8E-F0EEE6EA8986}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>0,10%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$S$6:$S$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.7415540219392903E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-6.9202836555831197E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.6617045951443602E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.70729481549075E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.4677655468735501E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-74F4-4649-AF8E-F0EEE6EA8986}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:v>0,05%</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$T$6:$T$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>5.7415540219392903E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.7105054312137601E-19</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>8.1370368257948704E-6</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>-4.4487537785892303E-6</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>-2.3954828038556201E-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Respuesta local experimental'!$B$6:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>365</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>695</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000F-74F4-4649-AF8E-F0EEE6EA8986}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="343793744"/>
+        <c:axId val="343788752"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="343793744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5.000000000000001E-3"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CL"/>
+                  <a:t>Horizontal</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-CL" baseline="0"/>
+                  <a:t> Strain</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-CL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="343788752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="343788752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-CL"/>
+                  <a:t>Height</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-CL" baseline="0"/>
+                  <a:t> (mm)</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-CL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="343793744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.7351108923884514"/>
+          <c:y val="0.27343503937007874"/>
+          <c:w val="0.1704446631671041"/>
+          <c:h val="0.49016695829687945"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1632,6 +5057,71 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -1930,13 +5420,13 @@
   <sheetData>
     <row r="7" spans="11:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="11:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K8" s="121" t="s">
+      <c r="K8" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="122"/>
-      <c r="M8" s="122"/>
-      <c r="N8" s="122"/>
-      <c r="O8" s="123"/>
+      <c r="L8" s="123"/>
+      <c r="M8" s="123"/>
+      <c r="N8" s="123"/>
+      <c r="O8" s="124"/>
     </row>
     <row r="9" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K9" s="2" t="s">
@@ -2662,13 +6152,13 @@
       <c r="F35" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="K35" s="121" t="s">
+      <c r="K35" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="L35" s="122"/>
-      <c r="M35" s="122"/>
-      <c r="N35" s="122"/>
-      <c r="O35" s="123"/>
+      <c r="L35" s="123"/>
+      <c r="M35" s="123"/>
+      <c r="N35" s="123"/>
+      <c r="O35" s="124"/>
       <c r="R35" s="51" t="s">
         <v>69</v>
       </c>
@@ -2699,12 +6189,12 @@
       <c r="K36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L36" s="124" t="s">
+      <c r="L36" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="M36" s="124"/>
-      <c r="N36" s="124"/>
-      <c r="O36" s="125"/>
+      <c r="M36" s="125"/>
+      <c r="N36" s="125"/>
+      <c r="O36" s="126"/>
       <c r="R36" s="51" t="s">
         <v>80</v>
       </c>
@@ -2905,17 +6395,17 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
-      <c r="D43" s="115" t="s">
+      <c r="D43" s="116" t="s">
         <v>41</v>
       </c>
-      <c r="E43" s="116"/>
+      <c r="E43" s="117"/>
       <c r="F43" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G43" s="115" t="s">
+      <c r="G43" s="116" t="s">
         <v>44</v>
       </c>
-      <c r="H43" s="116"/>
+      <c r="H43" s="117"/>
       <c r="I43" s="25" t="s">
         <v>37</v>
       </c>
@@ -2937,17 +6427,17 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
-      <c r="D44" s="117" t="s">
+      <c r="D44" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="E44" s="118"/>
+      <c r="E44" s="119"/>
       <c r="F44" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="G44" s="117" t="s">
+      <c r="G44" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="H44" s="118"/>
+      <c r="H44" s="119"/>
       <c r="I44" s="26" t="s">
         <v>49</v>
       </c>
@@ -3007,10 +6497,10 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="119" t="s">
+      <c r="A46" s="120" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="120"/>
+      <c r="B46" s="121"/>
       <c r="C46" s="19">
         <v>1</v>
       </c>
@@ -3037,7 +6527,7 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="113" t="s">
+      <c r="A47" s="114" t="s">
         <v>32</v>
       </c>
       <c r="B47" s="17" t="s">
@@ -3079,7 +6569,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="114"/>
+      <c r="A48" s="115"/>
       <c r="B48" s="28" t="s">
         <v>35</v>
       </c>
@@ -3119,7 +6609,7 @@
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="113" t="s">
+      <c r="A49" s="114" t="s">
         <v>33</v>
       </c>
       <c r="B49" s="32" t="s">
@@ -3161,7 +6651,7 @@
       </c>
     </row>
     <row r="50" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="114"/>
+      <c r="A50" s="115"/>
       <c r="B50" s="28" t="s">
         <v>35</v>
       </c>
@@ -3384,7 +6874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -3400,13 +6890,13 @@
   <sheetData>
     <row r="3" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="121" t="s">
+      <c r="C4" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="122"/>
-      <c r="E4" s="122"/>
-      <c r="F4" s="122"/>
-      <c r="G4" s="123"/>
+      <c r="D4" s="123"/>
+      <c r="E4" s="123"/>
+      <c r="F4" s="123"/>
+      <c r="G4" s="124"/>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
@@ -3911,8 +7401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:R35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4069,7 +7559,7 @@
         <v>0.75</v>
       </c>
       <c r="F7" s="72">
-        <f t="shared" ref="F6:F20" si="1">E7/$E$3</f>
+        <f t="shared" ref="F7:F20" si="1">E7/$E$3</f>
         <v>5</v>
       </c>
       <c r="G7" s="73">
@@ -4123,17 +7613,17 @@
         <f t="shared" ref="G9:G19" si="2">F9*4+G8</f>
         <v>100</v>
       </c>
-      <c r="J9" s="126" t="s">
+      <c r="J9" s="127" t="s">
         <v>122</v>
       </c>
-      <c r="K9" s="127"/>
-      <c r="L9" s="127"/>
-      <c r="M9" s="128"/>
-      <c r="O9" s="126" t="s">
+      <c r="K9" s="128"/>
+      <c r="L9" s="128"/>
+      <c r="M9" s="129"/>
+      <c r="O9" s="127" t="s">
         <v>112</v>
       </c>
-      <c r="P9" s="127"/>
-      <c r="Q9" s="128"/>
+      <c r="P9" s="128"/>
+      <c r="Q9" s="129"/>
     </row>
     <row r="10" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D10" s="71">
@@ -4151,14 +7641,14 @@
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
-      <c r="J10" s="126" t="s">
+      <c r="J10" s="127" t="s">
         <v>120</v>
       </c>
-      <c r="K10" s="128"/>
-      <c r="L10" s="126" t="s">
+      <c r="K10" s="129"/>
+      <c r="L10" s="127" t="s">
         <v>121</v>
       </c>
-      <c r="M10" s="128"/>
+      <c r="M10" s="129"/>
     </row>
     <row r="11" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D11" s="71">
@@ -4465,7 +7955,7 @@
         <v>13.5</v>
       </c>
       <c r="F18" s="72">
-        <f t="shared" si="1"/>
+        <f>E18/$E$3</f>
         <v>90</v>
       </c>
       <c r="G18" s="73">
@@ -4573,4 +8063,443 @@
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:T32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C3" s="127" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="128"/>
+      <c r="K3" s="129"/>
+      <c r="L3" s="127" t="s">
+        <v>127</v>
+      </c>
+      <c r="M3" s="128"/>
+      <c r="N3" s="128"/>
+      <c r="O3" s="128"/>
+      <c r="P3" s="128"/>
+      <c r="Q3" s="128"/>
+      <c r="R3" s="128"/>
+      <c r="S3" s="128"/>
+      <c r="T3" s="129"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C4" s="127" t="s">
+        <v>125</v>
+      </c>
+      <c r="D4" s="128"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="128"/>
+      <c r="G4" s="128"/>
+      <c r="H4" s="128"/>
+      <c r="I4" s="128"/>
+      <c r="J4" s="128"/>
+      <c r="K4" s="129"/>
+      <c r="L4" s="139" t="s">
+        <v>125</v>
+      </c>
+      <c r="M4" s="139"/>
+      <c r="N4" s="139"/>
+      <c r="O4" s="139"/>
+      <c r="P4" s="139"/>
+      <c r="Q4" s="139"/>
+      <c r="R4" s="139"/>
+      <c r="S4" s="139"/>
+      <c r="T4" s="140"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="133" t="s">
+        <v>124</v>
+      </c>
+      <c r="C5" s="138">
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="135">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E5" s="136">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F5" s="136">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G5" s="136">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H5" s="136">
+        <v>2E-3</v>
+      </c>
+      <c r="I5" s="136">
+        <v>1.5E-3</v>
+      </c>
+      <c r="J5" s="136">
+        <v>1E-3</v>
+      </c>
+      <c r="K5" s="137">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="L5" s="134">
+        <v>0.01</v>
+      </c>
+      <c r="M5" s="135">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="N5" s="136">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="O5" s="136">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="P5" s="136">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="Q5" s="136">
+        <v>2E-3</v>
+      </c>
+      <c r="R5" s="136">
+        <v>1.5E-3</v>
+      </c>
+      <c r="S5" s="136">
+        <v>1E-3</v>
+      </c>
+      <c r="T5" s="137">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="85">
+        <v>35</v>
+      </c>
+      <c r="C6" s="85">
+        <v>8.0158730158730101E-4</v>
+      </c>
+      <c r="D6" s="130">
+        <v>1.9047619047618999E-4</v>
+      </c>
+      <c r="E6" s="130">
+        <v>-2.38095238095242E-5</v>
+      </c>
+      <c r="F6" s="130">
+        <v>-4.7619047619048E-5</v>
+      </c>
+      <c r="G6" s="130">
+        <v>-3.9682539682540001E-5</v>
+      </c>
+      <c r="H6" s="130">
+        <v>-3.9682539682540001E-5</v>
+      </c>
+      <c r="I6" s="130">
+        <v>-2.38095238095242E-5</v>
+      </c>
+      <c r="J6" s="130">
+        <v>-3.9682539682540001E-5</v>
+      </c>
+      <c r="K6" s="86">
+        <v>-3.9682539682540001E-5</v>
+      </c>
+      <c r="L6" s="130">
+        <v>1.47976197266107E-3</v>
+      </c>
+      <c r="M6" s="130">
+        <v>8.4309587634745899E-4</v>
+      </c>
+      <c r="N6" s="130">
+        <v>4.4175744786022501E-4</v>
+      </c>
+      <c r="O6" s="130">
+        <v>2.6540428525256898E-5</v>
+      </c>
+      <c r="P6" s="130">
+        <v>5.7795775585084703E-6</v>
+      </c>
+      <c r="Q6" s="130">
+        <v>5.7415540219392903E-6</v>
+      </c>
+      <c r="R6" s="130">
+        <v>5.7415540219392903E-6</v>
+      </c>
+      <c r="S6" s="130">
+        <v>5.7415540219392903E-6</v>
+      </c>
+      <c r="T6" s="86">
+        <v>5.7415540219392903E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="85">
+        <f>B6+$P$32</f>
+        <v>200</v>
+      </c>
+      <c r="C7" s="85">
+        <v>2.6428571428571399E-3</v>
+      </c>
+      <c r="D7" s="130">
+        <v>1.84126984126984E-3</v>
+      </c>
+      <c r="E7" s="130">
+        <v>1.0873015873015799E-3</v>
+      </c>
+      <c r="F7" s="130">
+        <v>6.2698412698412604E-4</v>
+      </c>
+      <c r="G7" s="130">
+        <v>3.9682539682539601E-4</v>
+      </c>
+      <c r="H7" s="130">
+        <v>1.26984126984126E-4</v>
+      </c>
+      <c r="I7" s="130">
+        <v>1.58730158730155E-5</v>
+      </c>
+      <c r="J7" s="130">
+        <v>-2.38095238095242E-5</v>
+      </c>
+      <c r="K7" s="86">
+        <v>-3.1746031746032199E-5</v>
+      </c>
+      <c r="L7" s="130">
+        <v>2.2906138899979E-3</v>
+      </c>
+      <c r="M7" s="130">
+        <v>1.6955075191543499E-3</v>
+      </c>
+      <c r="N7" s="130">
+        <v>1.1141656685488301E-3</v>
+      </c>
+      <c r="O7" s="130">
+        <v>5.05180706857544E-4</v>
+      </c>
+      <c r="P7" s="130">
+        <v>3.25253331812391E-4</v>
+      </c>
+      <c r="Q7" s="130">
+        <v>1.31485389456073E-4</v>
+      </c>
+      <c r="R7" s="130">
+        <v>3.4601418277913698E-5</v>
+      </c>
+      <c r="S7" s="130">
+        <v>-6.9202836555831197E-6</v>
+      </c>
+      <c r="T7" s="88">
+        <v>-2.7105054312137601E-19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="85">
+        <f>B7+$P$32</f>
+        <v>365</v>
+      </c>
+      <c r="C8" s="85">
+        <v>1.95238095238095E-3</v>
+      </c>
+      <c r="D8" s="130">
+        <v>1.5238095238095199E-3</v>
+      </c>
+      <c r="E8" s="130">
+        <v>1.1587301587301501E-3</v>
+      </c>
+      <c r="F8" s="130">
+        <v>8.1746031746031704E-4</v>
+      </c>
+      <c r="G8" s="130">
+        <v>5.7936507936507905E-4</v>
+      </c>
+      <c r="H8" s="130">
+        <v>3.0952380952380901E-4</v>
+      </c>
+      <c r="I8" s="130">
+        <v>1.74603174603174E-4</v>
+      </c>
+      <c r="J8" s="130">
+        <v>5.5555555555555402E-5</v>
+      </c>
+      <c r="K8" s="86">
+        <v>-3.1746031746032199E-5</v>
+      </c>
+      <c r="L8" s="130">
+        <v>1.8004905036217401E-3</v>
+      </c>
+      <c r="M8" s="130">
+        <v>1.440673777068E-3</v>
+      </c>
+      <c r="N8" s="130">
+        <v>1.06002015247438E-3</v>
+      </c>
+      <c r="O8" s="130">
+        <v>6.72522291298313E-4</v>
+      </c>
+      <c r="P8" s="130">
+        <v>4.8567463259757698E-4</v>
+      </c>
+      <c r="Q8" s="130">
+        <v>2.78028099393524E-4</v>
+      </c>
+      <c r="R8" s="130">
+        <v>1.5346299359303301E-4</v>
+      </c>
+      <c r="S8" s="130">
+        <v>5.6617045951443602E-5</v>
+      </c>
+      <c r="T8" s="86">
+        <v>8.1370368257948704E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="85">
+        <f>B8+$P$32</f>
+        <v>530</v>
+      </c>
+      <c r="C9" s="85">
+        <v>1.4285714285714199E-3</v>
+      </c>
+      <c r="D9" s="130">
+        <v>1.1428571428571399E-3</v>
+      </c>
+      <c r="E9" s="130">
+        <v>9.2063492063492001E-4</v>
+      </c>
+      <c r="F9" s="130">
+        <v>6.8253968253968202E-4</v>
+      </c>
+      <c r="G9" s="130">
+        <v>4.8412698412698399E-4</v>
+      </c>
+      <c r="H9" s="130">
+        <v>2.6190476190476099E-4</v>
+      </c>
+      <c r="I9" s="130">
+        <v>1.3492063492063399E-4</v>
+      </c>
+      <c r="J9" s="130">
+        <v>3.9682539682539398E-5</v>
+      </c>
+      <c r="K9" s="86">
+        <v>-3.1746031746032199E-5</v>
+      </c>
+      <c r="L9" s="130">
+        <v>1.3450065590600499E-3</v>
+      </c>
+      <c r="M9" s="130">
+        <v>1.0820357801479101E-3</v>
+      </c>
+      <c r="N9" s="130">
+        <v>7.9138386661343303E-4</v>
+      </c>
+      <c r="O9" s="130">
+        <v>5.4917393866803503E-4</v>
+      </c>
+      <c r="P9" s="130">
+        <v>4.1076826555637902E-4</v>
+      </c>
+      <c r="Q9" s="130">
+        <v>2.37761174166809E-4</v>
+      </c>
+      <c r="R9" s="130">
+        <v>1.13196068366318E-4</v>
+      </c>
+      <c r="S9" s="130">
+        <v>3.70729481549075E-5</v>
+      </c>
+      <c r="T9" s="86">
+        <v>-4.4487537785892303E-6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="79">
+        <f>B9+$P$32</f>
+        <v>695</v>
+      </c>
+      <c r="C10" s="79">
+        <v>8.65079365079365E-4</v>
+      </c>
+      <c r="D10" s="131">
+        <v>7.0634920634920595E-4</v>
+      </c>
+      <c r="E10" s="131">
+        <v>5.8730158730158598E-4</v>
+      </c>
+      <c r="F10" s="131">
+        <v>4.4444444444444398E-4</v>
+      </c>
+      <c r="G10" s="131">
+        <v>3.0952380952380901E-4</v>
+      </c>
+      <c r="H10" s="131">
+        <v>1.19047619047618E-4</v>
+      </c>
+      <c r="I10" s="131">
+        <v>-7.9365079365082292E-6</v>
+      </c>
+      <c r="J10" s="131">
+        <v>-4.7619047619048E-5</v>
+      </c>
+      <c r="K10" s="132">
+        <v>-3.9682539682540001E-5</v>
+      </c>
+      <c r="L10" s="131">
+        <v>6.4043042643396203E-4</v>
+      </c>
+      <c r="M10" s="131">
+        <v>5.5046673891138596E-4</v>
+      </c>
+      <c r="N10" s="131">
+        <v>4.3282191676647801E-4</v>
+      </c>
+      <c r="O10" s="131">
+        <v>3.4285822924390102E-4</v>
+      </c>
+      <c r="P10" s="131">
+        <v>2.4597425806574199E-4</v>
+      </c>
+      <c r="Q10" s="131">
+        <v>1.21371128728682E-4</v>
+      </c>
+      <c r="R10" s="131">
+        <v>2.45251810870926E-5</v>
+      </c>
+      <c r="S10" s="131">
+        <v>-4.4677655468735501E-5</v>
+      </c>
+      <c r="T10" s="132">
+        <v>-2.3954828038556201E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="H22" s="113"/>
+    </row>
+    <row r="32" spans="8:16" x14ac:dyDescent="0.25">
+      <c r="P32">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C4:K4"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="L4:T4"/>
+    <mergeCell ref="L3:T3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se calculan las deformaciones horizontales por nivel
</commit_message>
<xml_diff>
--- a/Validacion/SW-T2-S3-4/Documentation/Documentacion SW-T2-S3-4.xlsx
+++ b/Validacion/SW-T2-S3-4/Documentation/Documentacion SW-T2-S3-4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="130">
   <si>
     <t>X coord [mm]</t>
   </si>
@@ -485,10 +485,7 @@
     <t>Espaciamiento LVDTs</t>
   </si>
   <si>
-    <t>Drift [%]</t>
-  </si>
-  <si>
-    <t>Load Step (3er ciclo)</t>
+    <t>DATA FOR MATLAB</t>
   </si>
 </sst>
 </file>
@@ -908,7 +905,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1218,60 +1215,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1282,15 +1225,83 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4805,8 +4816,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7212042" y="5097318"/>
-          <a:ext cx="4108275" cy="3278010"/>
+          <a:off x="7202517" y="5097318"/>
+          <a:ext cx="4101925" cy="3278010"/>
           <a:chOff x="7127376" y="4208318"/>
           <a:chExt cx="4108275" cy="3278010"/>
         </a:xfrm>
@@ -5084,15 +5095,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>280987</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>14287</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5115,14 +5126,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>21432</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>59532</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5409,8 +5420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A7:U72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5442,13 +5453,13 @@
   <sheetData>
     <row r="7" spans="11:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="11:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K8" s="121" t="s">
+      <c r="K8" s="137" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="122"/>
-      <c r="M8" s="122"/>
-      <c r="N8" s="122"/>
-      <c r="O8" s="123"/>
+      <c r="L8" s="138"/>
+      <c r="M8" s="138"/>
+      <c r="N8" s="138"/>
+      <c r="O8" s="139"/>
     </row>
     <row r="9" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K9" s="2" t="s">
@@ -5571,6 +5582,10 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
+      <c r="P13" s="1">
+        <f>N13/2</f>
+        <v>75</v>
+      </c>
       <c r="R13" s="51"/>
       <c r="S13" s="52" t="s">
         <v>13</v>
@@ -5599,6 +5614,10 @@
       <c r="O14" s="11">
         <f t="shared" si="1"/>
         <v>15</v>
+      </c>
+      <c r="P14" s="1">
+        <f>P13+150</f>
+        <v>225</v>
       </c>
       <c r="R14" s="51"/>
       <c r="S14" s="52"/>
@@ -5628,6 +5647,10 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
+      <c r="P15" s="1">
+        <f>P14+150</f>
+        <v>375</v>
+      </c>
       <c r="R15" s="51"/>
       <c r="S15" s="52" t="s">
         <v>16</v>
@@ -5656,6 +5679,10 @@
       <c r="O16" s="11">
         <f t="shared" si="1"/>
         <v>30</v>
+      </c>
+      <c r="P16" s="1">
+        <f t="shared" ref="P15:P33" si="2">P15+150</f>
+        <v>525</v>
       </c>
       <c r="R16" s="51"/>
       <c r="S16" s="52"/>
@@ -5685,6 +5712,10 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
+      <c r="P17" s="1">
+        <f t="shared" si="2"/>
+        <v>675</v>
+      </c>
       <c r="R17" s="51"/>
       <c r="S17" s="52" t="s">
         <v>17</v>
@@ -5713,6 +5744,10 @@
       <c r="O18" s="11">
         <f t="shared" si="1"/>
         <v>30</v>
+      </c>
+      <c r="P18" s="1">
+        <f t="shared" si="2"/>
+        <v>825</v>
       </c>
       <c r="R18" s="51"/>
       <c r="S18" s="52"/>
@@ -5742,6 +5777,10 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
+      <c r="P19" s="1">
+        <f t="shared" si="2"/>
+        <v>975</v>
+      </c>
       <c r="R19" s="51" t="s">
         <v>18</v>
       </c>
@@ -5772,6 +5811,10 @@
       <c r="O20" s="11">
         <f t="shared" si="1"/>
         <v>45</v>
+      </c>
+      <c r="P20" s="1">
+        <f t="shared" si="2"/>
+        <v>1125</v>
       </c>
       <c r="R20" s="51"/>
       <c r="S20" s="52"/>
@@ -5801,6 +5844,10 @@
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
+      <c r="P21" s="1">
+        <f t="shared" si="2"/>
+        <v>1275</v>
+      </c>
       <c r="R21" s="51" t="s">
         <v>20</v>
       </c>
@@ -5830,6 +5877,10 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
+      <c r="P22" s="1">
+        <f t="shared" si="2"/>
+        <v>1425</v>
+      </c>
       <c r="R22" s="53" t="s">
         <v>22</v>
       </c>
@@ -5859,6 +5910,10 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
+      <c r="P23" s="1">
+        <f t="shared" si="2"/>
+        <v>1575</v>
+      </c>
       <c r="R23" s="53" t="s">
         <v>23</v>
       </c>
@@ -5888,6 +5943,10 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
+      <c r="P24" s="1">
+        <f t="shared" si="2"/>
+        <v>1725</v>
+      </c>
       <c r="R24" s="51"/>
       <c r="S24" s="52" t="s">
         <v>26</v>
@@ -5915,6 +5974,10 @@
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
+      <c r="P25" s="1">
+        <f>P24+150</f>
+        <v>1875</v>
+      </c>
       <c r="R25" s="51"/>
       <c r="S25" s="52" t="s">
         <v>27</v>
@@ -5942,6 +6005,10 @@
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
+      <c r="P26" s="1">
+        <f t="shared" si="2"/>
+        <v>2025</v>
+      </c>
       <c r="R26" s="51"/>
       <c r="S26" s="52" t="s">
         <v>28</v>
@@ -5969,6 +6036,10 @@
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
+      <c r="P27" s="1">
+        <f t="shared" si="2"/>
+        <v>2175</v>
+      </c>
       <c r="R27" s="51"/>
       <c r="S27" s="52" t="s">
         <v>29</v>
@@ -5996,6 +6067,10 @@
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
+      <c r="P28" s="1">
+        <f t="shared" si="2"/>
+        <v>2325</v>
+      </c>
       <c r="R28" s="54"/>
       <c r="S28" s="40" t="s">
         <v>30</v>
@@ -6023,6 +6098,10 @@
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
+      <c r="P29" s="1">
+        <f t="shared" si="2"/>
+        <v>2475</v>
+      </c>
       <c r="R29" s="50" t="s">
         <v>60</v>
       </c>
@@ -6050,6 +6129,10 @@
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
+      <c r="P30" s="1">
+        <f t="shared" si="2"/>
+        <v>2625</v>
+      </c>
       <c r="R30" s="51" t="s">
         <v>62</v>
       </c>
@@ -6081,6 +6164,10 @@
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
+      <c r="P31" s="1">
+        <f t="shared" si="2"/>
+        <v>2775</v>
+      </c>
       <c r="R31" s="51" t="s">
         <v>64</v>
       </c>
@@ -6110,6 +6197,10 @@
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
+      <c r="P32" s="1">
+        <f t="shared" si="2"/>
+        <v>2925</v>
+      </c>
       <c r="S32" s="62" t="s">
         <v>86</v>
       </c>
@@ -6135,6 +6226,10 @@
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
+      <c r="P33" s="1">
+        <f t="shared" si="2"/>
+        <v>3075</v>
+      </c>
       <c r="R33" s="51" t="s">
         <v>66</v>
       </c>
@@ -6174,13 +6269,13 @@
       <c r="F35" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="K35" s="121" t="s">
+      <c r="K35" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="L35" s="122"/>
-      <c r="M35" s="122"/>
-      <c r="N35" s="122"/>
-      <c r="O35" s="123"/>
+      <c r="L35" s="138"/>
+      <c r="M35" s="138"/>
+      <c r="N35" s="138"/>
+      <c r="O35" s="139"/>
       <c r="R35" s="51" t="s">
         <v>69</v>
       </c>
@@ -6211,12 +6306,12 @@
       <c r="K36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L36" s="124" t="s">
+      <c r="L36" s="140" t="s">
         <v>8</v>
       </c>
-      <c r="M36" s="124"/>
-      <c r="N36" s="124"/>
-      <c r="O36" s="125"/>
+      <c r="M36" s="140"/>
+      <c r="N36" s="140"/>
+      <c r="O36" s="141"/>
       <c r="R36" s="51" t="s">
         <v>80</v>
       </c>
@@ -6417,17 +6512,17 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
-      <c r="D43" s="126" t="s">
+      <c r="D43" s="131" t="s">
         <v>41</v>
       </c>
-      <c r="E43" s="127"/>
+      <c r="E43" s="132"/>
       <c r="F43" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G43" s="126" t="s">
+      <c r="G43" s="131" t="s">
         <v>44</v>
       </c>
-      <c r="H43" s="127"/>
+      <c r="H43" s="132"/>
       <c r="I43" s="25" t="s">
         <v>37</v>
       </c>
@@ -6449,17 +6544,17 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
-      <c r="D44" s="128" t="s">
+      <c r="D44" s="133" t="s">
         <v>42</v>
       </c>
-      <c r="E44" s="129"/>
+      <c r="E44" s="134"/>
       <c r="F44" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="G44" s="128" t="s">
+      <c r="G44" s="133" t="s">
         <v>45</v>
       </c>
-      <c r="H44" s="129"/>
+      <c r="H44" s="134"/>
       <c r="I44" s="26" t="s">
         <v>49</v>
       </c>
@@ -6519,10 +6614,10 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="132" t="s">
+      <c r="A46" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="133"/>
+      <c r="B46" s="136"/>
       <c r="C46" s="19">
         <v>1</v>
       </c>
@@ -6549,7 +6644,7 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="130" t="s">
+      <c r="A47" s="129" t="s">
         <v>32</v>
       </c>
       <c r="B47" s="17" t="s">
@@ -6591,7 +6686,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="131"/>
+      <c r="A48" s="130"/>
       <c r="B48" s="28" t="s">
         <v>35</v>
       </c>
@@ -6631,7 +6726,7 @@
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="130" t="s">
+      <c r="A49" s="129" t="s">
         <v>33</v>
       </c>
       <c r="B49" s="32" t="s">
@@ -6673,7 +6768,7 @@
       </c>
     </row>
     <row r="50" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="131"/>
+      <c r="A50" s="130"/>
       <c r="B50" s="28" t="s">
         <v>35</v>
       </c>
@@ -6874,16 +6969,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="K8:O8"/>
+    <mergeCell ref="L36:O36"/>
+    <mergeCell ref="K35:O35"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="G43:H43"/>
     <mergeCell ref="G44:H44"/>
     <mergeCell ref="A46:B46"/>
-    <mergeCell ref="K8:O8"/>
-    <mergeCell ref="L36:O36"/>
-    <mergeCell ref="K35:O35"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -6912,13 +7007,13 @@
   <sheetData>
     <row r="3" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="121" t="s">
+      <c r="C4" s="137" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="122"/>
-      <c r="E4" s="122"/>
-      <c r="F4" s="122"/>
-      <c r="G4" s="123"/>
+      <c r="D4" s="138"/>
+      <c r="E4" s="138"/>
+      <c r="F4" s="138"/>
+      <c r="G4" s="139"/>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
@@ -7423,8 +7518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:R35"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7546,11 +7641,11 @@
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" s="139">
+      <c r="D6" s="121">
         <v>0.05</v>
       </c>
-      <c r="E6" s="140">
-        <f t="shared" ref="E6:E20" si="0">$E$2*D6/100</f>
+      <c r="E6" s="122">
+        <f>$E$2*D6/100</f>
         <v>0.375</v>
       </c>
       <c r="F6" s="72">
@@ -7573,11 +7668,11 @@
       </c>
     </row>
     <row r="7" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D7" s="139">
+      <c r="D7" s="121">
         <v>0.1</v>
       </c>
-      <c r="E7" s="140">
-        <f t="shared" si="0"/>
+      <c r="E7" s="122">
+        <f t="shared" ref="E6:E20" si="0">$E$2*D7/100</f>
         <v>0.75</v>
       </c>
       <c r="F7" s="72">
@@ -7603,10 +7698,10 @@
       <c r="C8">
         <v>15</v>
       </c>
-      <c r="D8" s="139">
+      <c r="D8" s="121">
         <v>0.15</v>
       </c>
-      <c r="E8" s="140">
+      <c r="E8" s="122">
         <f t="shared" si="0"/>
         <v>1.125</v>
       </c>
@@ -7620,10 +7715,10 @@
       </c>
     </row>
     <row r="9" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D9" s="139">
+      <c r="D9" s="121">
         <v>0.2</v>
       </c>
-      <c r="E9" s="140">
+      <c r="E9" s="122">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
@@ -7635,23 +7730,23 @@
         <f t="shared" ref="G9:G19" si="2">F9*4+G8</f>
         <v>100</v>
       </c>
-      <c r="J9" s="134" t="s">
+      <c r="J9" s="142" t="s">
         <v>122</v>
       </c>
-      <c r="K9" s="135"/>
-      <c r="L9" s="135"/>
-      <c r="M9" s="136"/>
-      <c r="O9" s="134" t="s">
+      <c r="K9" s="143"/>
+      <c r="L9" s="143"/>
+      <c r="M9" s="144"/>
+      <c r="O9" s="142" t="s">
         <v>112</v>
       </c>
-      <c r="P9" s="135"/>
-      <c r="Q9" s="136"/>
+      <c r="P9" s="143"/>
+      <c r="Q9" s="144"/>
     </row>
     <row r="10" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D10" s="139">
+      <c r="D10" s="121">
         <v>0.3</v>
       </c>
-      <c r="E10" s="140">
+      <c r="E10" s="122">
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
@@ -7663,20 +7758,20 @@
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
-      <c r="J10" s="134" t="s">
+      <c r="J10" s="142" t="s">
         <v>120</v>
       </c>
-      <c r="K10" s="136"/>
-      <c r="L10" s="134" t="s">
+      <c r="K10" s="144"/>
+      <c r="L10" s="142" t="s">
         <v>121</v>
       </c>
-      <c r="M10" s="136"/>
+      <c r="M10" s="144"/>
     </row>
     <row r="11" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D11" s="139">
+      <c r="D11" s="121">
         <v>0.4</v>
       </c>
-      <c r="E11" s="140">
+      <c r="E11" s="122">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -7714,10 +7809,10 @@
       <c r="C12" t="s">
         <v>101</v>
       </c>
-      <c r="D12" s="141">
+      <c r="D12" s="123">
         <v>0.6</v>
       </c>
-      <c r="E12" s="142">
+      <c r="E12" s="124">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
@@ -7757,10 +7852,10 @@
       </c>
     </row>
     <row r="13" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D13" s="139">
+      <c r="D13" s="121">
         <v>0.8</v>
       </c>
-      <c r="E13" s="140">
+      <c r="E13" s="122">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -7800,10 +7895,10 @@
       </c>
     </row>
     <row r="14" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="D14" s="139">
+      <c r="D14" s="121">
         <v>1</v>
       </c>
-      <c r="E14" s="140">
+      <c r="E14" s="122">
         <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
@@ -8089,10 +8184,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:T39"/>
+  <dimension ref="B3:T38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X30" sqref="X30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8101,52 +8196,52 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="134" t="s">
+      <c r="C3" s="142" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135"/>
-      <c r="K3" s="136"/>
-      <c r="L3" s="134" t="s">
+      <c r="D3" s="143"/>
+      <c r="E3" s="143"/>
+      <c r="F3" s="143"/>
+      <c r="G3" s="143"/>
+      <c r="H3" s="143"/>
+      <c r="I3" s="143"/>
+      <c r="J3" s="143"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="142" t="s">
         <v>127</v>
       </c>
-      <c r="M3" s="135"/>
-      <c r="N3" s="135"/>
-      <c r="O3" s="135"/>
-      <c r="P3" s="135"/>
-      <c r="Q3" s="135"/>
-      <c r="R3" s="135"/>
-      <c r="S3" s="135"/>
-      <c r="T3" s="136"/>
+      <c r="M3" s="143"/>
+      <c r="N3" s="143"/>
+      <c r="O3" s="143"/>
+      <c r="P3" s="143"/>
+      <c r="Q3" s="143"/>
+      <c r="R3" s="143"/>
+      <c r="S3" s="143"/>
+      <c r="T3" s="144"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C4" s="134" t="s">
+      <c r="C4" s="142" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="135"/>
-      <c r="E4" s="135"/>
-      <c r="F4" s="135"/>
-      <c r="G4" s="135"/>
-      <c r="H4" s="135"/>
-      <c r="I4" s="135"/>
-      <c r="J4" s="135"/>
-      <c r="K4" s="136"/>
-      <c r="L4" s="137" t="s">
+      <c r="D4" s="143"/>
+      <c r="E4" s="143"/>
+      <c r="F4" s="143"/>
+      <c r="G4" s="143"/>
+      <c r="H4" s="143"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="143"/>
+      <c r="K4" s="144"/>
+      <c r="L4" s="145" t="s">
         <v>125</v>
       </c>
-      <c r="M4" s="137"/>
-      <c r="N4" s="137"/>
-      <c r="O4" s="137"/>
-      <c r="P4" s="137"/>
-      <c r="Q4" s="137"/>
-      <c r="R4" s="137"/>
-      <c r="S4" s="137"/>
-      <c r="T4" s="138"/>
+      <c r="M4" s="145"/>
+      <c r="N4" s="145"/>
+      <c r="O4" s="145"/>
+      <c r="P4" s="145"/>
+      <c r="Q4" s="145"/>
+      <c r="R4" s="145"/>
+      <c r="S4" s="145"/>
+      <c r="T4" s="146"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="115" t="s">
@@ -8271,58 +8366,58 @@
         <f>B6+$C$12</f>
         <v>200</v>
       </c>
-      <c r="C7" s="144">
+      <c r="C7" s="125">
         <v>2.6428571428571399E-3</v>
       </c>
-      <c r="D7" s="145">
+      <c r="D7" s="126">
         <v>1.84126984126984E-3</v>
       </c>
-      <c r="E7" s="145">
+      <c r="E7" s="126">
         <v>1.0873015873015799E-3</v>
       </c>
-      <c r="F7" s="145">
+      <c r="F7" s="126">
         <v>6.2698412698412604E-4</v>
       </c>
-      <c r="G7" s="145">
+      <c r="G7" s="126">
         <v>3.9682539682539601E-4</v>
       </c>
-      <c r="H7" s="145">
+      <c r="H7" s="126">
         <v>1.26984126984126E-4</v>
       </c>
-      <c r="I7" s="145">
+      <c r="I7" s="126">
         <v>1.58730158730155E-5</v>
       </c>
-      <c r="J7" s="145">
+      <c r="J7" s="126">
         <v>-2.38095238095242E-5</v>
       </c>
-      <c r="K7" s="146">
+      <c r="K7" s="127">
         <v>-3.1746031746032199E-5</v>
       </c>
-      <c r="L7" s="145">
+      <c r="L7" s="126">
         <v>2.2906138899979E-3</v>
       </c>
-      <c r="M7" s="145">
+      <c r="M7" s="126">
         <v>1.6955075191543499E-3</v>
       </c>
-      <c r="N7" s="145">
+      <c r="N7" s="126">
         <v>1.1141656685488301E-3</v>
       </c>
-      <c r="O7" s="145">
+      <c r="O7" s="126">
         <v>5.05180706857544E-4</v>
       </c>
-      <c r="P7" s="145">
+      <c r="P7" s="126">
         <v>3.25253331812391E-4</v>
       </c>
-      <c r="Q7" s="145">
+      <c r="Q7" s="126">
         <v>1.31485389456073E-4</v>
       </c>
-      <c r="R7" s="145">
+      <c r="R7" s="126">
         <v>3.4601418277913698E-5</v>
       </c>
-      <c r="S7" s="145">
+      <c r="S7" s="126">
         <v>-6.9202836555831197E-6</v>
       </c>
-      <c r="T7" s="147">
+      <c r="T7" s="128">
         <v>-2.7105054312137601E-19</v>
       </c>
     </row>
@@ -8517,162 +8612,459 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="H22" s="111"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C28" s="155" t="s">
+        <v>129</v>
+      </c>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
+      <c r="K28" s="156"/>
+      <c r="L28" s="156"/>
+      <c r="M28" s="156"/>
+      <c r="N28" s="156"/>
+      <c r="O28" s="156"/>
+      <c r="P28" s="156"/>
+      <c r="Q28" s="156"/>
+      <c r="R28" s="156"/>
+      <c r="S28" s="156"/>
+      <c r="T28" s="157"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C29" s="142" t="s">
         <v>126</v>
       </c>
-      <c r="E29" t="s">
+      <c r="D29" s="143"/>
+      <c r="E29" s="143"/>
+      <c r="F29" s="143"/>
+      <c r="G29" s="143"/>
+      <c r="H29" s="143"/>
+      <c r="I29" s="143"/>
+      <c r="J29" s="143"/>
+      <c r="K29" s="144"/>
+      <c r="L29" s="142" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="C30" s="69" t="s">
-        <v>90</v>
-      </c>
-      <c r="D30" s="143" t="s">
-        <v>130</v>
-      </c>
+      <c r="M29" s="143"/>
+      <c r="N29" s="143"/>
+      <c r="O29" s="143"/>
+      <c r="P29" s="143"/>
+      <c r="Q29" s="143"/>
+      <c r="R29" s="143"/>
+      <c r="S29" s="143"/>
+      <c r="T29" s="144"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C30" s="142" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="143"/>
       <c r="E30" s="143"/>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="44">
-        <v>0.05</v>
-      </c>
-      <c r="C31" s="44">
-        <v>0.375</v>
-      </c>
-      <c r="D31">
-        <v>68</v>
-      </c>
-      <c r="E31">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="44">
-        <v>0.1</v>
-      </c>
-      <c r="C32" s="44">
-        <v>0.75</v>
-      </c>
-      <c r="D32">
-        <v>131</v>
-      </c>
-      <c r="E32">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="44">
-        <v>0.15</v>
-      </c>
-      <c r="C33" s="44">
-        <v>1.125</v>
-      </c>
-      <c r="D33">
-        <v>284</v>
-      </c>
-      <c r="E33">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="44">
-        <v>0.2</v>
-      </c>
-      <c r="C34" s="44">
-        <v>1.5</v>
-      </c>
-      <c r="D34">
-        <v>422</v>
-      </c>
-      <c r="E34">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="44">
-        <v>0.3</v>
-      </c>
-      <c r="C35" s="44">
-        <v>2.25</v>
-      </c>
-      <c r="D35">
-        <v>590</v>
-      </c>
-      <c r="E35">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="44">
-        <v>0.4</v>
-      </c>
-      <c r="C36" s="44">
-        <v>3</v>
-      </c>
-      <c r="D36">
-        <v>818</v>
-      </c>
-      <c r="E36">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="44">
-        <v>0.6</v>
-      </c>
-      <c r="C37" s="44">
-        <v>4.5</v>
-      </c>
-      <c r="D37">
-        <v>1151</v>
-      </c>
-      <c r="E37">
-        <v>1211</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="44">
-        <v>0.8</v>
-      </c>
-      <c r="C38" s="44">
-        <v>6</v>
-      </c>
-      <c r="D38">
-        <v>1604</v>
-      </c>
-      <c r="E38">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="44">
-        <v>1</v>
-      </c>
-      <c r="C39" s="44">
-        <v>7.5</v>
-      </c>
-      <c r="D39">
-        <v>2177</v>
-      </c>
-      <c r="E39">
-        <v>2277</v>
+      <c r="F30" s="143"/>
+      <c r="G30" s="143"/>
+      <c r="H30" s="143"/>
+      <c r="I30" s="143"/>
+      <c r="J30" s="143"/>
+      <c r="K30" s="144"/>
+      <c r="L30" s="145" t="s">
+        <v>125</v>
+      </c>
+      <c r="M30" s="145"/>
+      <c r="N30" s="145"/>
+      <c r="O30" s="145"/>
+      <c r="P30" s="145"/>
+      <c r="Q30" s="145"/>
+      <c r="R30" s="145"/>
+      <c r="S30" s="145"/>
+      <c r="T30" s="146"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="115" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="151">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D31" s="117">
+        <v>1E-3</v>
+      </c>
+      <c r="E31" s="118">
+        <v>1.5E-3</v>
+      </c>
+      <c r="F31" s="118">
+        <v>2E-3</v>
+      </c>
+      <c r="G31" s="118">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H31" s="118">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I31" s="118">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J31" s="118">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="K31" s="153">
+        <v>0.01</v>
+      </c>
+      <c r="L31" s="151">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="M31" s="117">
+        <v>1E-3</v>
+      </c>
+      <c r="N31" s="118">
+        <v>1.5E-3</v>
+      </c>
+      <c r="O31" s="118">
+        <v>2E-3</v>
+      </c>
+      <c r="P31" s="118">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="Q31" s="118">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="R31" s="118">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="S31" s="118">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="T31" s="150">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="101">
+        <v>35</v>
+      </c>
+      <c r="C32" s="83">
+        <v>-3.9682539682540001E-5</v>
+      </c>
+      <c r="D32" s="112">
+        <v>-3.9682539682540001E-5</v>
+      </c>
+      <c r="E32" s="112">
+        <v>-2.38095238095242E-5</v>
+      </c>
+      <c r="F32" s="112">
+        <v>-3.9682539682540001E-5</v>
+      </c>
+      <c r="G32" s="112">
+        <v>-3.9682539682540001E-5</v>
+      </c>
+      <c r="H32" s="112">
+        <v>-4.7619047619048E-5</v>
+      </c>
+      <c r="I32" s="112">
+        <v>-2.38095238095242E-5</v>
+      </c>
+      <c r="J32" s="112">
+        <v>1.9047619047618999E-4</v>
+      </c>
+      <c r="K32" s="112">
+        <v>8.0158730158730101E-4</v>
+      </c>
+      <c r="L32" s="83">
+        <v>5.7415540219392903E-6</v>
+      </c>
+      <c r="M32" s="112">
+        <v>5.7415540219392903E-6</v>
+      </c>
+      <c r="N32" s="112">
+        <v>5.7415540219392903E-6</v>
+      </c>
+      <c r="O32" s="112">
+        <v>5.7415540219392903E-6</v>
+      </c>
+      <c r="P32" s="112">
+        <v>5.7795775585084703E-6</v>
+      </c>
+      <c r="Q32" s="112">
+        <v>2.6540428525256898E-5</v>
+      </c>
+      <c r="R32" s="112">
+        <v>4.4175744786022501E-4</v>
+      </c>
+      <c r="S32" s="112">
+        <v>8.4309587634745899E-4</v>
+      </c>
+      <c r="T32" s="84">
+        <v>1.47976197266107E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="103">
+        <f>B32+$C$38</f>
+        <v>200</v>
+      </c>
+      <c r="C33" s="147">
+        <v>-3.1746031746032199E-5</v>
+      </c>
+      <c r="D33" s="148">
+        <v>-2.38095238095242E-5</v>
+      </c>
+      <c r="E33" s="148">
+        <v>1.58730158730155E-5</v>
+      </c>
+      <c r="F33" s="148">
+        <v>1.26984126984126E-4</v>
+      </c>
+      <c r="G33" s="148">
+        <v>3.9682539682539601E-4</v>
+      </c>
+      <c r="H33" s="148">
+        <v>6.2698412698412604E-4</v>
+      </c>
+      <c r="I33" s="148">
+        <v>1.0873015873015799E-3</v>
+      </c>
+      <c r="J33" s="148">
+        <v>1.84126984126984E-3</v>
+      </c>
+      <c r="K33" s="148">
+        <v>2.6428571428571399E-3</v>
+      </c>
+      <c r="L33" s="152">
+        <v>-2.7105054312137601E-19</v>
+      </c>
+      <c r="M33" s="148">
+        <v>-6.9202836555831197E-6</v>
+      </c>
+      <c r="N33" s="148">
+        <v>3.4601418277913698E-5</v>
+      </c>
+      <c r="O33" s="148">
+        <v>1.31485389456073E-4</v>
+      </c>
+      <c r="P33" s="148">
+        <v>3.25253331812391E-4</v>
+      </c>
+      <c r="Q33" s="148">
+        <v>5.05180706857544E-4</v>
+      </c>
+      <c r="R33" s="148">
+        <v>1.1141656685488301E-3</v>
+      </c>
+      <c r="S33" s="148">
+        <v>1.6955075191543499E-3</v>
+      </c>
+      <c r="T33" s="149">
+        <v>2.2906138899979E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="103">
+        <f>B33+$C$38</f>
+        <v>365</v>
+      </c>
+      <c r="C34" s="83">
+        <v>-3.1746031746032199E-5</v>
+      </c>
+      <c r="D34" s="112">
+        <v>5.5555555555555402E-5</v>
+      </c>
+      <c r="E34" s="112">
+        <v>1.74603174603174E-4</v>
+      </c>
+      <c r="F34" s="112">
+        <v>3.0952380952380901E-4</v>
+      </c>
+      <c r="G34" s="112">
+        <v>5.7936507936507905E-4</v>
+      </c>
+      <c r="H34" s="112">
+        <v>8.1746031746031704E-4</v>
+      </c>
+      <c r="I34" s="112">
+        <v>1.1587301587301501E-3</v>
+      </c>
+      <c r="J34" s="112">
+        <v>1.5238095238095199E-3</v>
+      </c>
+      <c r="K34" s="112">
+        <v>1.95238095238095E-3</v>
+      </c>
+      <c r="L34" s="83">
+        <v>8.1370368257948704E-6</v>
+      </c>
+      <c r="M34" s="112">
+        <v>5.6617045951443602E-5</v>
+      </c>
+      <c r="N34" s="112">
+        <v>1.5346299359303301E-4</v>
+      </c>
+      <c r="O34" s="112">
+        <v>2.78028099393524E-4</v>
+      </c>
+      <c r="P34" s="112">
+        <v>4.8567463259757698E-4</v>
+      </c>
+      <c r="Q34" s="112">
+        <v>6.72522291298313E-4</v>
+      </c>
+      <c r="R34" s="112">
+        <v>1.06002015247438E-3</v>
+      </c>
+      <c r="S34" s="112">
+        <v>1.440673777068E-3</v>
+      </c>
+      <c r="T34" s="84">
+        <v>1.8004905036217401E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="103">
+        <f>B34+$C$38</f>
+        <v>530</v>
+      </c>
+      <c r="C35" s="83">
+        <v>-3.1746031746032199E-5</v>
+      </c>
+      <c r="D35" s="112">
+        <v>3.9682539682539398E-5</v>
+      </c>
+      <c r="E35" s="112">
+        <v>1.3492063492063399E-4</v>
+      </c>
+      <c r="F35" s="112">
+        <v>2.6190476190476099E-4</v>
+      </c>
+      <c r="G35" s="112">
+        <v>4.8412698412698399E-4</v>
+      </c>
+      <c r="H35" s="112">
+        <v>6.8253968253968202E-4</v>
+      </c>
+      <c r="I35" s="112">
+        <v>9.2063492063492001E-4</v>
+      </c>
+      <c r="J35" s="112">
+        <v>1.1428571428571399E-3</v>
+      </c>
+      <c r="K35" s="112">
+        <v>1.4285714285714199E-3</v>
+      </c>
+      <c r="L35" s="83">
+        <v>-4.4487537785892303E-6</v>
+      </c>
+      <c r="M35" s="112">
+        <v>3.70729481549075E-5</v>
+      </c>
+      <c r="N35" s="112">
+        <v>1.13196068366318E-4</v>
+      </c>
+      <c r="O35" s="112">
+        <v>2.37761174166809E-4</v>
+      </c>
+      <c r="P35" s="112">
+        <v>4.1076826555637902E-4</v>
+      </c>
+      <c r="Q35" s="112">
+        <v>5.4917393866803503E-4</v>
+      </c>
+      <c r="R35" s="112">
+        <v>7.9138386661343303E-4</v>
+      </c>
+      <c r="S35" s="112">
+        <v>1.0820357801479101E-3</v>
+      </c>
+      <c r="T35" s="84">
+        <v>1.3450065590600499E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="154">
+        <f>B35+$C$38</f>
+        <v>695</v>
+      </c>
+      <c r="C36" s="77">
+        <v>-3.9682539682540001E-5</v>
+      </c>
+      <c r="D36" s="113">
+        <v>-4.7619047619048E-5</v>
+      </c>
+      <c r="E36" s="113">
+        <v>-7.9365079365082292E-6</v>
+      </c>
+      <c r="F36" s="113">
+        <v>1.19047619047618E-4</v>
+      </c>
+      <c r="G36" s="113">
+        <v>3.0952380952380901E-4</v>
+      </c>
+      <c r="H36" s="113">
+        <v>4.4444444444444398E-4</v>
+      </c>
+      <c r="I36" s="113">
+        <v>5.8730158730158598E-4</v>
+      </c>
+      <c r="J36" s="113">
+        <v>7.0634920634920595E-4</v>
+      </c>
+      <c r="K36" s="113">
+        <v>8.65079365079365E-4</v>
+      </c>
+      <c r="L36" s="77">
+        <v>-2.3954828038556201E-5</v>
+      </c>
+      <c r="M36" s="113">
+        <v>-4.4677655468735501E-5</v>
+      </c>
+      <c r="N36" s="113">
+        <v>2.45251810870926E-5</v>
+      </c>
+      <c r="O36" s="113">
+        <v>1.21371128728682E-4</v>
+      </c>
+      <c r="P36" s="113">
+        <v>2.4597425806574199E-4</v>
+      </c>
+      <c r="Q36" s="113">
+        <v>3.4285822924390102E-4</v>
+      </c>
+      <c r="R36" s="113">
+        <v>4.3282191676647801E-4</v>
+      </c>
+      <c r="S36" s="113">
+        <v>5.5046673891138596E-4</v>
+      </c>
+      <c r="T36" s="114">
+        <v>6.4043042643396203E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38">
+        <v>165</v>
+      </c>
+      <c r="D38" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="C29:K29"/>
+    <mergeCell ref="L29:T29"/>
+    <mergeCell ref="C30:K30"/>
+    <mergeCell ref="L30:T30"/>
+    <mergeCell ref="C28:T28"/>
     <mergeCell ref="C4:K4"/>
     <mergeCell ref="C3:K3"/>
     <mergeCell ref="L4:T4"/>
     <mergeCell ref="L3:T3"/>
-    <mergeCell ref="D30:E30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Se agrega script para calculo de energia disipada
</commit_message>
<xml_diff>
--- a/Validacion/SW-T2-S3-4/Documentation/Documentacion SW-T2-S3-4.xlsx
+++ b/Validacion/SW-T2-S3-4/Documentation/Documentacion SW-T2-S3-4.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" activeTab="3"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="3" r:id="rId2"/>
     <sheet name=" Drift y Factor de daño  " sheetId="2" r:id="rId3"/>
     <sheet name="Resp local exp y analitica " sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="132">
   <si>
     <t>X coord [mm]</t>
   </si>
@@ -486,6 +487,12 @@
   </si>
   <si>
     <t>DATA FOR MATLAB</t>
+  </si>
+  <si>
+    <t>Load Step inicio drift</t>
+  </si>
+  <si>
+    <t>Load Step fin drift</t>
   </si>
 </sst>
 </file>
@@ -1231,60 +1238,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1293,6 +1246,60 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5681,7 +5688,7 @@
         <v>30</v>
       </c>
       <c r="P16" s="1">
-        <f t="shared" ref="P15:P33" si="2">P15+150</f>
+        <f t="shared" ref="P16:P33" si="2">P15+150</f>
         <v>525</v>
       </c>
       <c r="R16" s="51"/>
@@ -6512,17 +6519,17 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
-      <c r="D43" s="131" t="s">
+      <c r="D43" s="142" t="s">
         <v>41</v>
       </c>
-      <c r="E43" s="132"/>
+      <c r="E43" s="143"/>
       <c r="F43" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="G43" s="131" t="s">
+      <c r="G43" s="142" t="s">
         <v>44</v>
       </c>
-      <c r="H43" s="132"/>
+      <c r="H43" s="143"/>
       <c r="I43" s="25" t="s">
         <v>37</v>
       </c>
@@ -6544,17 +6551,17 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="16"/>
-      <c r="D44" s="133" t="s">
+      <c r="D44" s="144" t="s">
         <v>42</v>
       </c>
-      <c r="E44" s="134"/>
+      <c r="E44" s="145"/>
       <c r="F44" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="G44" s="133" t="s">
+      <c r="G44" s="144" t="s">
         <v>45</v>
       </c>
-      <c r="H44" s="134"/>
+      <c r="H44" s="145"/>
       <c r="I44" s="26" t="s">
         <v>49</v>
       </c>
@@ -6614,10 +6621,10 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="135" t="s">
+      <c r="A46" s="148" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="136"/>
+      <c r="B46" s="149"/>
       <c r="C46" s="19">
         <v>1</v>
       </c>
@@ -6644,7 +6651,7 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="129" t="s">
+      <c r="A47" s="146" t="s">
         <v>32</v>
       </c>
       <c r="B47" s="17" t="s">
@@ -6686,7 +6693,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="130"/>
+      <c r="A48" s="147"/>
       <c r="B48" s="28" t="s">
         <v>35</v>
       </c>
@@ -6726,7 +6733,7 @@
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="129" t="s">
+      <c r="A49" s="146" t="s">
         <v>33</v>
       </c>
       <c r="B49" s="32" t="s">
@@ -6768,7 +6775,7 @@
       </c>
     </row>
     <row r="50" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="130"/>
+      <c r="A50" s="147"/>
       <c r="B50" s="28" t="s">
         <v>35</v>
       </c>
@@ -6969,16 +6976,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="A46:B46"/>
     <mergeCell ref="K8:O8"/>
     <mergeCell ref="L36:O36"/>
     <mergeCell ref="K35:O35"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="D44:E44"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="A46:B46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -7518,8 +7525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:R35"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7672,7 +7679,7 @@
         <v>0.1</v>
       </c>
       <c r="E7" s="122">
-        <f t="shared" ref="E6:E20" si="0">$E$2*D7/100</f>
+        <f t="shared" ref="E7:E20" si="0">$E$2*D7/100</f>
         <v>0.75</v>
       </c>
       <c r="F7" s="72">
@@ -7730,17 +7737,17 @@
         <f t="shared" ref="G9:G19" si="2">F9*4+G8</f>
         <v>100</v>
       </c>
-      <c r="J9" s="142" t="s">
+      <c r="J9" s="150" t="s">
         <v>122</v>
       </c>
-      <c r="K9" s="143"/>
-      <c r="L9" s="143"/>
-      <c r="M9" s="144"/>
-      <c r="O9" s="142" t="s">
+      <c r="K9" s="151"/>
+      <c r="L9" s="151"/>
+      <c r="M9" s="152"/>
+      <c r="O9" s="150" t="s">
         <v>112</v>
       </c>
-      <c r="P9" s="143"/>
-      <c r="Q9" s="144"/>
+      <c r="P9" s="151"/>
+      <c r="Q9" s="152"/>
     </row>
     <row r="10" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D10" s="121">
@@ -7758,14 +7765,14 @@
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
-      <c r="J10" s="142" t="s">
+      <c r="J10" s="150" t="s">
         <v>120</v>
       </c>
-      <c r="K10" s="144"/>
-      <c r="L10" s="142" t="s">
+      <c r="K10" s="152"/>
+      <c r="L10" s="150" t="s">
         <v>121</v>
       </c>
-      <c r="M10" s="144"/>
+      <c r="M10" s="152"/>
     </row>
     <row r="11" spans="3:18" x14ac:dyDescent="0.25">
       <c r="D11" s="121">
@@ -8186,7 +8193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="X30" sqref="X30"/>
     </sheetView>
   </sheetViews>
@@ -8196,52 +8203,52 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="142" t="s">
+      <c r="C3" s="150" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="143"/>
-      <c r="E3" s="143"/>
-      <c r="F3" s="143"/>
-      <c r="G3" s="143"/>
-      <c r="H3" s="143"/>
-      <c r="I3" s="143"/>
-      <c r="J3" s="143"/>
-      <c r="K3" s="144"/>
-      <c r="L3" s="142" t="s">
+      <c r="D3" s="151"/>
+      <c r="E3" s="151"/>
+      <c r="F3" s="151"/>
+      <c r="G3" s="151"/>
+      <c r="H3" s="151"/>
+      <c r="I3" s="151"/>
+      <c r="J3" s="151"/>
+      <c r="K3" s="152"/>
+      <c r="L3" s="150" t="s">
         <v>127</v>
       </c>
-      <c r="M3" s="143"/>
-      <c r="N3" s="143"/>
-      <c r="O3" s="143"/>
-      <c r="P3" s="143"/>
-      <c r="Q3" s="143"/>
-      <c r="R3" s="143"/>
-      <c r="S3" s="143"/>
-      <c r="T3" s="144"/>
+      <c r="M3" s="151"/>
+      <c r="N3" s="151"/>
+      <c r="O3" s="151"/>
+      <c r="P3" s="151"/>
+      <c r="Q3" s="151"/>
+      <c r="R3" s="151"/>
+      <c r="S3" s="151"/>
+      <c r="T3" s="152"/>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C4" s="142" t="s">
+      <c r="C4" s="150" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="143"/>
-      <c r="E4" s="143"/>
-      <c r="F4" s="143"/>
-      <c r="G4" s="143"/>
-      <c r="H4" s="143"/>
-      <c r="I4" s="143"/>
-      <c r="J4" s="143"/>
-      <c r="K4" s="144"/>
-      <c r="L4" s="145" t="s">
+      <c r="D4" s="151"/>
+      <c r="E4" s="151"/>
+      <c r="F4" s="151"/>
+      <c r="G4" s="151"/>
+      <c r="H4" s="151"/>
+      <c r="I4" s="151"/>
+      <c r="J4" s="151"/>
+      <c r="K4" s="152"/>
+      <c r="L4" s="153" t="s">
         <v>125</v>
       </c>
-      <c r="M4" s="145"/>
-      <c r="N4" s="145"/>
-      <c r="O4" s="145"/>
-      <c r="P4" s="145"/>
-      <c r="Q4" s="145"/>
-      <c r="R4" s="145"/>
-      <c r="S4" s="145"/>
-      <c r="T4" s="146"/>
+      <c r="M4" s="153"/>
+      <c r="N4" s="153"/>
+      <c r="O4" s="153"/>
+      <c r="P4" s="153"/>
+      <c r="Q4" s="153"/>
+      <c r="R4" s="153"/>
+      <c r="S4" s="153"/>
+      <c r="T4" s="154"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B5" s="115" t="s">
@@ -8638,58 +8645,58 @@
       <c r="T28" s="157"/>
     </row>
     <row r="29" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C29" s="142" t="s">
+      <c r="C29" s="150" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="143"/>
-      <c r="E29" s="143"/>
-      <c r="F29" s="143"/>
-      <c r="G29" s="143"/>
-      <c r="H29" s="143"/>
-      <c r="I29" s="143"/>
-      <c r="J29" s="143"/>
-      <c r="K29" s="144"/>
-      <c r="L29" s="142" t="s">
+      <c r="D29" s="151"/>
+      <c r="E29" s="151"/>
+      <c r="F29" s="151"/>
+      <c r="G29" s="151"/>
+      <c r="H29" s="151"/>
+      <c r="I29" s="151"/>
+      <c r="J29" s="151"/>
+      <c r="K29" s="152"/>
+      <c r="L29" s="150" t="s">
         <v>127</v>
       </c>
-      <c r="M29" s="143"/>
-      <c r="N29" s="143"/>
-      <c r="O29" s="143"/>
-      <c r="P29" s="143"/>
-      <c r="Q29" s="143"/>
-      <c r="R29" s="143"/>
-      <c r="S29" s="143"/>
-      <c r="T29" s="144"/>
+      <c r="M29" s="151"/>
+      <c r="N29" s="151"/>
+      <c r="O29" s="151"/>
+      <c r="P29" s="151"/>
+      <c r="Q29" s="151"/>
+      <c r="R29" s="151"/>
+      <c r="S29" s="151"/>
+      <c r="T29" s="152"/>
     </row>
     <row r="30" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C30" s="142" t="s">
+      <c r="C30" s="150" t="s">
         <v>125</v>
       </c>
-      <c r="D30" s="143"/>
-      <c r="E30" s="143"/>
-      <c r="F30" s="143"/>
-      <c r="G30" s="143"/>
-      <c r="H30" s="143"/>
-      <c r="I30" s="143"/>
-      <c r="J30" s="143"/>
-      <c r="K30" s="144"/>
-      <c r="L30" s="145" t="s">
+      <c r="D30" s="151"/>
+      <c r="E30" s="151"/>
+      <c r="F30" s="151"/>
+      <c r="G30" s="151"/>
+      <c r="H30" s="151"/>
+      <c r="I30" s="151"/>
+      <c r="J30" s="151"/>
+      <c r="K30" s="152"/>
+      <c r="L30" s="153" t="s">
         <v>125</v>
       </c>
-      <c r="M30" s="145"/>
-      <c r="N30" s="145"/>
-      <c r="O30" s="145"/>
-      <c r="P30" s="145"/>
-      <c r="Q30" s="145"/>
-      <c r="R30" s="145"/>
-      <c r="S30" s="145"/>
-      <c r="T30" s="146"/>
+      <c r="M30" s="153"/>
+      <c r="N30" s="153"/>
+      <c r="O30" s="153"/>
+      <c r="P30" s="153"/>
+      <c r="Q30" s="153"/>
+      <c r="R30" s="153"/>
+      <c r="S30" s="153"/>
+      <c r="T30" s="154"/>
     </row>
     <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" s="115" t="s">
         <v>124</v>
       </c>
-      <c r="C31" s="151">
+      <c r="C31" s="133">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="D31" s="117">
@@ -8713,10 +8720,10 @@
       <c r="J31" s="118">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="K31" s="153">
+      <c r="K31" s="135">
         <v>0.01</v>
       </c>
-      <c r="L31" s="151">
+      <c r="L31" s="133">
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="M31" s="117">
@@ -8740,7 +8747,7 @@
       <c r="S31" s="118">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="T31" s="150">
+      <c r="T31" s="132">
         <v>0.01</v>
       </c>
     </row>
@@ -8808,58 +8815,58 @@
         <f>B32+$C$38</f>
         <v>200</v>
       </c>
-      <c r="C33" s="147">
+      <c r="C33" s="129">
         <v>-3.1746031746032199E-5</v>
       </c>
-      <c r="D33" s="148">
+      <c r="D33" s="130">
         <v>-2.38095238095242E-5</v>
       </c>
-      <c r="E33" s="148">
+      <c r="E33" s="130">
         <v>1.58730158730155E-5</v>
       </c>
-      <c r="F33" s="148">
+      <c r="F33" s="130">
         <v>1.26984126984126E-4</v>
       </c>
-      <c r="G33" s="148">
+      <c r="G33" s="130">
         <v>3.9682539682539601E-4</v>
       </c>
-      <c r="H33" s="148">
+      <c r="H33" s="130">
         <v>6.2698412698412604E-4</v>
       </c>
-      <c r="I33" s="148">
+      <c r="I33" s="130">
         <v>1.0873015873015799E-3</v>
       </c>
-      <c r="J33" s="148">
+      <c r="J33" s="130">
         <v>1.84126984126984E-3</v>
       </c>
-      <c r="K33" s="148">
+      <c r="K33" s="130">
         <v>2.6428571428571399E-3</v>
       </c>
-      <c r="L33" s="152">
+      <c r="L33" s="134">
         <v>-2.7105054312137601E-19</v>
       </c>
-      <c r="M33" s="148">
+      <c r="M33" s="130">
         <v>-6.9202836555831197E-6</v>
       </c>
-      <c r="N33" s="148">
+      <c r="N33" s="130">
         <v>3.4601418277913698E-5</v>
       </c>
-      <c r="O33" s="148">
+      <c r="O33" s="130">
         <v>1.31485389456073E-4</v>
       </c>
-      <c r="P33" s="148">
+      <c r="P33" s="130">
         <v>3.25253331812391E-4</v>
       </c>
-      <c r="Q33" s="148">
+      <c r="Q33" s="130">
         <v>5.05180706857544E-4</v>
       </c>
-      <c r="R33" s="148">
+      <c r="R33" s="130">
         <v>1.1141656685488301E-3</v>
       </c>
-      <c r="S33" s="148">
+      <c r="S33" s="130">
         <v>1.6955075191543499E-3</v>
       </c>
-      <c r="T33" s="149">
+      <c r="T33" s="131">
         <v>2.2906138899979E-3</v>
       </c>
     </row>
@@ -8984,7 +8991,7 @@
       </c>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B36" s="154">
+      <c r="B36" s="136">
         <f>B35+$C$38</f>
         <v>695</v>
       </c>
@@ -9056,17 +9063,260 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C4:K4"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="L4:T4"/>
+    <mergeCell ref="L3:T3"/>
     <mergeCell ref="C29:K29"/>
     <mergeCell ref="L29:T29"/>
     <mergeCell ref="C30:K30"/>
     <mergeCell ref="L30:T30"/>
     <mergeCell ref="C28:T28"/>
-    <mergeCell ref="C4:K4"/>
-    <mergeCell ref="C3:K3"/>
-    <mergeCell ref="L4:T4"/>
-    <mergeCell ref="L3:T3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:F19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>0.05</v>
+      </c>
+      <c r="D5">
+        <v>0.375</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0.1</v>
+      </c>
+      <c r="D6">
+        <v>0.75</v>
+      </c>
+      <c r="E6">
+        <v>83</v>
+      </c>
+      <c r="F6">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>0.15</v>
+      </c>
+      <c r="D7">
+        <v>1.125</v>
+      </c>
+      <c r="E7">
+        <v>146</v>
+      </c>
+      <c r="F7">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>0.2</v>
+      </c>
+      <c r="D8">
+        <v>1.5</v>
+      </c>
+      <c r="E8">
+        <v>329</v>
+      </c>
+      <c r="F8">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>0.3</v>
+      </c>
+      <c r="D9">
+        <v>2.25</v>
+      </c>
+      <c r="E9">
+        <v>452</v>
+      </c>
+      <c r="F9">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>0.4</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>635</v>
+      </c>
+      <c r="F10">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>0.6</v>
+      </c>
+      <c r="D11">
+        <v>4.5</v>
+      </c>
+      <c r="E11">
+        <v>878</v>
+      </c>
+      <c r="F11">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>0.8</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>1241</v>
+      </c>
+      <c r="F12">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>7.5</v>
+      </c>
+      <c r="E13">
+        <v>1724</v>
+      </c>
+      <c r="F13">
+        <v>2327</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>1.2</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+      <c r="E14">
+        <v>2327</v>
+      </c>
+      <c r="F14">
+        <v>3050</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>1.4</v>
+      </c>
+      <c r="D15">
+        <v>10.5</v>
+      </c>
+      <c r="E15">
+        <v>3050</v>
+      </c>
+      <c r="F15">
+        <v>3893</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>1.6</v>
+      </c>
+      <c r="D16">
+        <v>12</v>
+      </c>
+      <c r="E16">
+        <v>3893</v>
+      </c>
+      <c r="F16">
+        <v>4856</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>1.8</v>
+      </c>
+      <c r="D17">
+        <v>13.5</v>
+      </c>
+      <c r="E17">
+        <v>4856</v>
+      </c>
+      <c r="F17">
+        <v>5939</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>5939</v>
+      </c>
+      <c r="F18">
+        <v>7142</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>2.4</v>
+      </c>
+      <c r="D19">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>7142</v>
+      </c>
+      <c r="F19">
+        <v>8585</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se modifica esquema iterativo y discretizacion
</commit_message>
<xml_diff>
--- a/Validacion/SW-T2-S3-4/Documentation/Documentacion SW-T2-S3-4.xlsx
+++ b/Validacion/SW-T2-S3-4/Documentation/Documentacion SW-T2-S3-4.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Ejemplos\Validacion\SW-T2-S3-4\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maryj\Documents\GitHub\Ejemplos\Validacion\SW-T2-S3-4\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E7CA71-8CCE-42BC-B4E1-2DAA2B0ED46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="4"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
     <sheet name="Resp local exp y analitica " sheetId="4" r:id="rId4"/>
     <sheet name="Energia Disipada" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,12 +40,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Maria Jose Nuñez</author>
   </authors>
   <commentList>
-    <comment ref="F37" authorId="0" shapeId="0">
+    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -68,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S38" authorId="0" shapeId="0">
+    <comment ref="S38" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -97,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="136">
   <si>
     <t>X coord [mm]</t>
   </si>
@@ -499,12 +500,18 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>REGULARIZACIÓN DE LA RESPUESTA SEGÚN LARGO DE ROTULA PLASTICA</t>
+  </si>
+  <si>
+    <t>Lp = 2,0tw</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -918,7 +925,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1198,13 +1205,36 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1220,30 +1250,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1268,6 +1274,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1277,12 +1286,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1304,7 +1309,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2188,7 +2193,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2226,7 +2231,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1487595088"/>
@@ -2305,7 +2310,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2343,7 +2348,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1487598416"/>
@@ -2397,7 +2402,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2427,7 +2432,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2441,7 +2446,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3325,7 +3330,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3363,7 +3368,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="343788752"/>
@@ -3442,7 +3447,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="es-CL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -3480,7 +3485,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-CL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="343793744"/>
@@ -3532,7 +3537,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-CL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3562,7 +3567,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-CL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4698,7 +4703,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>305996</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>134128</xdr:rowOff>
+      <xdr:rowOff>130318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4740,9 +4745,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>808034</xdr:colOff>
+      <xdr:colOff>815654</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>56742</xdr:rowOff>
+      <xdr:rowOff>60552</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5449,51 +5454,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A7:U50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A7:U103"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I91" sqref="I91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="3" width="19.140625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="11.42578125" style="1"/>
-    <col min="6" max="6" width="16.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" style="1" customWidth="1"/>
-    <col min="10" max="11" width="11.42578125" style="1"/>
-    <col min="12" max="12" width="13.42578125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.28515625" style="1" customWidth="1"/>
-    <col min="16" max="17" width="11.42578125" style="1"/>
-    <col min="18" max="18" width="48.7109375" style="15" customWidth="1"/>
-    <col min="19" max="19" width="31.5703125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="18.140625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" style="1" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" style="1"/>
-    <col min="23" max="23" width="18.5703125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="18.28515625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="19.7109375" style="1" customWidth="1"/>
-    <col min="26" max="26" width="21.42578125" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="2" width="11.44140625" style="1"/>
+    <col min="3" max="3" width="19.109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="11.44140625" style="1"/>
+    <col min="6" max="6" width="16.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5546875" style="1" customWidth="1"/>
+    <col min="10" max="11" width="11.44140625" style="1"/>
+    <col min="12" max="12" width="13.44140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" style="1" customWidth="1"/>
+    <col min="16" max="17" width="11.44140625" style="1"/>
+    <col min="18" max="18" width="48.6640625" style="15" customWidth="1"/>
+    <col min="19" max="19" width="31.5546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="18.109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="15.88671875" style="1" customWidth="1"/>
+    <col min="22" max="22" width="11.44140625" style="1"/>
+    <col min="23" max="23" width="18.5546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="18.33203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="19.6640625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="21.44140625" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="11:21" ht="14.45" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="11:21" ht="14.45" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K8" s="118" t="s">
+    <row r="7" spans="11:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="11:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="125" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="119"/>
-      <c r="M8" s="119"/>
-      <c r="N8" s="119"/>
-      <c r="O8" s="120"/>
-    </row>
-    <row r="9" spans="11:21" ht="13.9" x14ac:dyDescent="0.25">
+      <c r="L8" s="126"/>
+      <c r="M8" s="126"/>
+      <c r="N8" s="126"/>
+      <c r="O8" s="127"/>
+    </row>
+    <row r="9" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K9" s="2" t="s">
         <v>6</v>
       </c>
@@ -5510,7 +5515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="11:21" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="10" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K10" s="4">
         <v>1</v>
       </c>
@@ -5537,7 +5542,7 @@
       <c r="T10" s="16"/>
       <c r="U10" s="17"/>
     </row>
-    <row r="11" spans="11:21" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="11" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K11" s="4">
         <v>2</v>
       </c>
@@ -5568,7 +5573,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="11:21" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="12" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K12" s="4">
         <v>3</v>
       </c>
@@ -5596,7 +5601,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="11:21" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="13" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K13" s="4">
         <v>4</v>
       </c>
@@ -5629,7 +5634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="11:21" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="14" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K14" s="4">
         <v>5</v>
       </c>
@@ -5661,7 +5666,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="11:21" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="15" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K15" s="4">
         <v>6</v>
       </c>
@@ -5694,7 +5699,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="11:21" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="16" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K16" s="4">
         <v>7</v>
       </c>
@@ -5726,7 +5731,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="11:21" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="17" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K17" s="4">
         <v>8</v>
       </c>
@@ -5759,7 +5764,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="11:21" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="18" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K18" s="4">
         <v>9</v>
       </c>
@@ -5826,7 +5831,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="11:21" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="20" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K20" s="4">
         <v>11</v>
       </c>
@@ -5891,7 +5896,7 @@
       </c>
       <c r="U21" s="21"/>
     </row>
-    <row r="22" spans="11:21" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="22" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K22" s="4">
         <v>13</v>
       </c>
@@ -5924,7 +5929,7 @@
       </c>
       <c r="U22" s="21"/>
     </row>
-    <row r="23" spans="11:21" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="23" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K23" s="4">
         <v>14</v>
       </c>
@@ -5957,7 +5962,7 @@
       </c>
       <c r="U23" s="21"/>
     </row>
-    <row r="24" spans="11:21" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="24" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K24" s="4">
         <v>15</v>
       </c>
@@ -5988,7 +5993,7 @@
       </c>
       <c r="U24" s="21"/>
     </row>
-    <row r="25" spans="11:21" ht="13.9" x14ac:dyDescent="0.25">
+    <row r="25" spans="11:21" x14ac:dyDescent="0.25">
       <c r="K25" s="51">
         <v>16</v>
       </c>
@@ -6240,7 +6245,7 @@
         <v>-5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K33" s="5">
         <v>24</v>
       </c>
@@ -6276,7 +6281,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="S34" s="49" t="s">
         <v>87</v>
       </c>
@@ -6288,7 +6293,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="22" t="s">
         <v>51</v>
       </c>
@@ -6301,13 +6306,13 @@
       <c r="F35" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="K35" s="118" t="s">
+      <c r="K35" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="L35" s="119"/>
-      <c r="M35" s="119"/>
-      <c r="N35" s="119"/>
-      <c r="O35" s="120"/>
+      <c r="L35" s="126"/>
+      <c r="M35" s="126"/>
+      <c r="N35" s="126"/>
+      <c r="O35" s="127"/>
       <c r="R35" s="38" t="s">
         <v>69</v>
       </c>
@@ -6338,12 +6343,12 @@
       <c r="K36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L36" s="121" t="s">
+      <c r="L36" s="128" t="s">
         <v>8</v>
       </c>
-      <c r="M36" s="121"/>
-      <c r="N36" s="121"/>
-      <c r="O36" s="122"/>
+      <c r="M36" s="128"/>
+      <c r="N36" s="128"/>
+      <c r="O36" s="129"/>
       <c r="R36" s="38" t="s">
         <v>80</v>
       </c>
@@ -6544,17 +6549,17 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="15"/>
-      <c r="D43" s="123" t="s">
+      <c r="D43" s="119" t="s">
         <v>41</v>
       </c>
-      <c r="E43" s="124"/>
+      <c r="E43" s="120"/>
       <c r="F43" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="G43" s="123" t="s">
+      <c r="G43" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="H43" s="124"/>
+      <c r="H43" s="120"/>
       <c r="I43" s="24" t="s">
         <v>37</v>
       </c>
@@ -6576,17 +6581,17 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="15"/>
-      <c r="D44" s="125" t="s">
+      <c r="D44" s="121" t="s">
         <v>42</v>
       </c>
-      <c r="E44" s="126"/>
+      <c r="E44" s="122"/>
       <c r="F44" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="G44" s="125" t="s">
+      <c r="G44" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="H44" s="126"/>
+      <c r="H44" s="122"/>
       <c r="I44" s="25" t="s">
         <v>49</v>
       </c>
@@ -6646,10 +6651,10 @@
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A46" s="129" t="s">
+      <c r="A46" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="130"/>
+      <c r="B46" s="124"/>
       <c r="C46" s="18">
         <v>1</v>
       </c>
@@ -6676,7 +6681,7 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="127" t="s">
+      <c r="A47" s="117" t="s">
         <v>32</v>
       </c>
       <c r="B47" s="16" t="s">
@@ -6718,7 +6723,7 @@
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="128"/>
+      <c r="A48" s="118"/>
       <c r="B48" s="27" t="s">
         <v>35</v>
       </c>
@@ -6758,7 +6763,7 @@
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" s="127" t="s">
+      <c r="A49" s="117" t="s">
         <v>33</v>
       </c>
       <c r="B49" s="16" t="s">
@@ -6799,8 +6804,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="128"/>
+    <row r="50" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="118"/>
       <c r="B50" s="27" t="s">
         <v>35</v>
       </c>
@@ -6839,18 +6844,532 @@
         <v>23</v>
       </c>
     </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" s="142" t="s">
+        <v>134</v>
+      </c>
+      <c r="B73" s="142"/>
+      <c r="C73" s="142"/>
+      <c r="D73" s="142"/>
+      <c r="E73" s="142"/>
+      <c r="F73" s="142"/>
+      <c r="G73" s="142"/>
+      <c r="H73" s="142"/>
+      <c r="I73" s="142"/>
+      <c r="J73" s="142"/>
+      <c r="K73" s="142"/>
+      <c r="L73" s="142"/>
+      <c r="M73" s="142"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B75" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C75" s="1">
+        <f>2*120</f>
+        <v>240</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B78" s="125" t="s">
+        <v>4</v>
+      </c>
+      <c r="C78" s="126"/>
+      <c r="D78" s="126"/>
+      <c r="E78" s="126"/>
+      <c r="F78" s="127"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B79" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F79" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B80" s="4">
+        <v>1</v>
+      </c>
+      <c r="C80" s="1">
+        <v>0</v>
+      </c>
+      <c r="D80" s="8">
+        <f>C80/10</f>
+        <v>0</v>
+      </c>
+      <c r="E80" s="1">
+        <v>0</v>
+      </c>
+      <c r="F80" s="11">
+        <f>E80/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" s="4">
+        <v>2</v>
+      </c>
+      <c r="C81" s="1">
+        <v>750</v>
+      </c>
+      <c r="D81" s="8">
+        <f t="shared" ref="D81:D103" si="3">C81/10</f>
+        <v>75</v>
+      </c>
+      <c r="E81" s="1">
+        <v>0</v>
+      </c>
+      <c r="F81" s="11">
+        <f t="shared" ref="F81:F103" si="4">E81/10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B82" s="4">
+        <v>3</v>
+      </c>
+      <c r="C82" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D82" s="8">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="E82" s="1">
+        <v>0</v>
+      </c>
+      <c r="F82" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B83" s="4">
+        <v>4</v>
+      </c>
+      <c r="C83" s="1">
+        <v>0</v>
+      </c>
+      <c r="D83" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E83" s="1">
+        <v>150</v>
+      </c>
+      <c r="F83" s="11">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" s="4">
+        <v>5</v>
+      </c>
+      <c r="C84" s="1">
+        <v>750</v>
+      </c>
+      <c r="D84" s="8">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="E84" s="1">
+        <v>150</v>
+      </c>
+      <c r="F84" s="11">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B85" s="4">
+        <v>6</v>
+      </c>
+      <c r="C85" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D85" s="8">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="E85" s="1">
+        <v>150</v>
+      </c>
+      <c r="F85" s="11">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B86" s="4">
+        <v>7</v>
+      </c>
+      <c r="C86" s="1">
+        <v>0</v>
+      </c>
+      <c r="D86" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E86" s="1">
+        <v>300</v>
+      </c>
+      <c r="F86" s="11">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B87" s="4">
+        <v>8</v>
+      </c>
+      <c r="C87" s="1">
+        <v>750</v>
+      </c>
+      <c r="D87" s="8">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="E87" s="1">
+        <v>300</v>
+      </c>
+      <c r="F87" s="11">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B88" s="4">
+        <v>9</v>
+      </c>
+      <c r="C88" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D88" s="8">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="E88" s="1">
+        <v>300</v>
+      </c>
+      <c r="F88" s="11">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B89" s="4">
+        <v>10</v>
+      </c>
+      <c r="C89" s="1">
+        <v>0</v>
+      </c>
+      <c r="D89" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E89" s="1">
+        <v>450</v>
+      </c>
+      <c r="F89" s="11">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B90" s="4">
+        <v>11</v>
+      </c>
+      <c r="C90" s="1">
+        <v>750</v>
+      </c>
+      <c r="D90" s="8">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="E90" s="1">
+        <v>450</v>
+      </c>
+      <c r="F90" s="11">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B91" s="4">
+        <v>12</v>
+      </c>
+      <c r="C91" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D91" s="8">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="E91" s="1">
+        <v>450</v>
+      </c>
+      <c r="F91" s="11">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B92" s="4">
+        <v>13</v>
+      </c>
+      <c r="C92" s="1">
+        <v>0</v>
+      </c>
+      <c r="D92" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E92" s="1">
+        <v>600</v>
+      </c>
+      <c r="F92" s="11">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B93" s="4">
+        <v>14</v>
+      </c>
+      <c r="C93" s="1">
+        <v>750</v>
+      </c>
+      <c r="D93" s="8">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="E93" s="1">
+        <v>600</v>
+      </c>
+      <c r="F93" s="11">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B94" s="4">
+        <v>15</v>
+      </c>
+      <c r="C94" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D94" s="8">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="E94" s="1">
+        <v>600</v>
+      </c>
+      <c r="F94" s="11">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B95" s="51">
+        <v>16</v>
+      </c>
+      <c r="C95" s="52">
+        <v>0</v>
+      </c>
+      <c r="D95" s="53">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E95" s="52">
+        <v>750</v>
+      </c>
+      <c r="F95" s="54">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B96" s="4">
+        <v>17</v>
+      </c>
+      <c r="C96" s="1">
+        <v>750</v>
+      </c>
+      <c r="D96" s="8">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="E96" s="1">
+        <v>750</v>
+      </c>
+      <c r="F96" s="11">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B97" s="4">
+        <v>18</v>
+      </c>
+      <c r="C97" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D97" s="8">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="E97" s="1">
+        <v>750</v>
+      </c>
+      <c r="F97" s="11">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B98" s="4">
+        <v>19</v>
+      </c>
+      <c r="C98" s="1">
+        <v>0</v>
+      </c>
+      <c r="D98" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E98" s="1">
+        <v>950</v>
+      </c>
+      <c r="F98" s="11">
+        <f t="shared" si="4"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B99" s="4">
+        <v>20</v>
+      </c>
+      <c r="C99" s="1">
+        <v>750</v>
+      </c>
+      <c r="D99" s="8">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="E99" s="1">
+        <v>950</v>
+      </c>
+      <c r="F99" s="11">
+        <f t="shared" si="4"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B100" s="4">
+        <v>21</v>
+      </c>
+      <c r="C100" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D100" s="8">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="E100" s="1">
+        <v>950</v>
+      </c>
+      <c r="F100" s="11">
+        <f t="shared" si="4"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B101" s="4">
+        <v>22</v>
+      </c>
+      <c r="C101" s="1">
+        <v>0</v>
+      </c>
+      <c r="D101" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E101" s="1">
+        <v>1150</v>
+      </c>
+      <c r="F101" s="11">
+        <f t="shared" si="4"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B102" s="4">
+        <v>23</v>
+      </c>
+      <c r="C102" s="1">
+        <v>750</v>
+      </c>
+      <c r="D102" s="8">
+        <f t="shared" si="3"/>
+        <v>75</v>
+      </c>
+      <c r="E102" s="1">
+        <v>1150</v>
+      </c>
+      <c r="F102" s="11">
+        <f t="shared" si="4"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="5">
+        <v>24</v>
+      </c>
+      <c r="C103" s="6">
+        <v>1500</v>
+      </c>
+      <c r="D103" s="9">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="E103" s="6">
+        <v>1150</v>
+      </c>
+      <c r="F103" s="12">
+        <f t="shared" si="4"/>
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="A73:M73"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="K8:O8"/>
+    <mergeCell ref="L36:O36"/>
+    <mergeCell ref="K35:O35"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="G43:H43"/>
     <mergeCell ref="G44:H44"/>
     <mergeCell ref="A46:B46"/>
-    <mergeCell ref="K8:O8"/>
-    <mergeCell ref="L36:O36"/>
-    <mergeCell ref="K35:O35"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -6860,34 +7379,34 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C3:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" style="36"/>
-    <col min="3" max="3" width="10.85546875" style="36" customWidth="1"/>
+    <col min="1" max="2" width="11.44140625" style="36"/>
+    <col min="3" max="3" width="10.88671875" style="36" customWidth="1"/>
     <col min="4" max="4" width="22" style="36" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" style="36" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="36" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="36"/>
+    <col min="5" max="5" width="21.109375" style="36" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" style="36" customWidth="1"/>
+    <col min="7" max="16384" width="11.44140625" style="36"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="118" t="s">
+    <row r="3" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="125" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="120"/>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D4" s="126"/>
+      <c r="E4" s="126"/>
+      <c r="F4" s="126"/>
+      <c r="G4" s="127"/>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C5" s="2" t="s">
         <v>6</v>
       </c>
@@ -6904,7 +7423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" s="4">
         <v>1</v>
       </c>
@@ -6923,7 +7442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C7" s="4">
         <v>2</v>
       </c>
@@ -6942,7 +7461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C8" s="4">
         <v>3</v>
       </c>
@@ -6961,7 +7480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C9" s="4">
         <v>4</v>
       </c>
@@ -6980,7 +7499,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C10" s="4">
         <v>5</v>
       </c>
@@ -6999,7 +7518,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C11" s="4">
         <v>6</v>
       </c>
@@ -7018,7 +7537,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C12" s="4">
         <v>7</v>
       </c>
@@ -7038,7 +7557,7 @@
         <v>36.75</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C13" s="4">
         <v>8</v>
       </c>
@@ -7058,7 +7577,7 @@
         <v>36.75</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C14" s="4">
         <v>9</v>
       </c>
@@ -7078,7 +7597,7 @@
         <v>36.75</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C15" s="4">
         <v>10</v>
       </c>
@@ -7098,7 +7617,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C16" s="4">
         <v>11</v>
       </c>
@@ -7118,7 +7637,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C17" s="4">
         <v>12</v>
       </c>
@@ -7138,7 +7657,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C18" s="4">
         <v>13</v>
       </c>
@@ -7158,7 +7677,7 @@
         <v>62.25</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C19" s="4">
         <v>14</v>
       </c>
@@ -7178,7 +7697,7 @@
         <v>62.25</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C20" s="4">
         <v>15</v>
       </c>
@@ -7198,7 +7717,7 @@
         <v>62.25</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C21" s="4">
         <v>16</v>
       </c>
@@ -7218,7 +7737,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C22" s="4">
         <v>17</v>
       </c>
@@ -7238,7 +7757,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C23" s="4">
         <v>18</v>
       </c>
@@ -7258,7 +7777,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C24" s="4">
         <v>19</v>
       </c>
@@ -7278,7 +7797,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C25" s="4">
         <v>20</v>
       </c>
@@ -7298,7 +7817,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C26" s="4">
         <v>21</v>
       </c>
@@ -7318,7 +7837,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C27" s="4">
         <v>22</v>
       </c>
@@ -7338,7 +7857,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C28" s="4">
         <v>23</v>
       </c>
@@ -7358,7 +7877,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C29" s="5">
         <v>24</v>
       </c>
@@ -7387,89 +7906,89 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="C2:R35"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="7.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" customWidth="1"/>
+    <col min="7" max="7" width="20.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="36" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" style="36" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="14" width="5.7109375" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" customWidth="1"/>
-    <col min="18" max="18" width="22.85546875" customWidth="1"/>
-    <col min="19" max="19" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" style="36" customWidth="1"/>
+    <col min="11" max="11" width="14.109375" style="36" customWidth="1"/>
+    <col min="12" max="12" width="13.44140625" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" customWidth="1"/>
+    <col min="14" max="14" width="5.6640625" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" customWidth="1"/>
+    <col min="17" max="17" width="15.5546875" customWidth="1"/>
+    <col min="18" max="18" width="22.88671875" customWidth="1"/>
+    <col min="19" max="19" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D2" s="62" t="s">
         <v>89</v>
       </c>
@@ -7477,7 +7996,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="3" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D3" s="63" t="s">
         <v>92</v>
       </c>
@@ -7489,7 +8008,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D5" s="55" t="s">
         <v>59</v>
       </c>
@@ -7509,7 +8028,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>5</v>
       </c>
@@ -7539,7 +8058,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="7" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D7" s="103">
         <v>0.1</v>
       </c>
@@ -7566,7 +8085,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="8" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>15</v>
       </c>
@@ -7586,7 +8105,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D9" s="103">
         <v>0.2</v>
       </c>
@@ -7602,19 +8121,19 @@
         <f t="shared" ref="G9:G19" si="2">F9*4+G8</f>
         <v>100</v>
       </c>
-      <c r="J9" s="131" t="s">
+      <c r="J9" s="130" t="s">
         <v>122</v>
       </c>
-      <c r="K9" s="132"/>
-      <c r="L9" s="132"/>
-      <c r="M9" s="133"/>
-      <c r="O9" s="131" t="s">
+      <c r="K9" s="131"/>
+      <c r="L9" s="131"/>
+      <c r="M9" s="132"/>
+      <c r="O9" s="130" t="s">
         <v>112</v>
       </c>
-      <c r="P9" s="132"/>
-      <c r="Q9" s="133"/>
-    </row>
-    <row r="10" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="P9" s="131"/>
+      <c r="Q9" s="132"/>
+    </row>
+    <row r="10" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D10" s="103">
         <v>0.3</v>
       </c>
@@ -7630,16 +8149,16 @@
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
-      <c r="J10" s="131" t="s">
+      <c r="J10" s="130" t="s">
         <v>120</v>
       </c>
-      <c r="K10" s="133"/>
-      <c r="L10" s="131" t="s">
+      <c r="K10" s="132"/>
+      <c r="L10" s="130" t="s">
         <v>121</v>
       </c>
-      <c r="M10" s="133"/>
-    </row>
-    <row r="11" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="M10" s="132"/>
+    </row>
+    <row r="11" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D11" s="103">
         <v>0.4</v>
       </c>
@@ -7677,7 +8196,7 @@
         <v>-2E-3</v>
       </c>
     </row>
-    <row r="12" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:18" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>101</v>
       </c>
@@ -7723,7 +8242,7 @@
         <v>1.6034840853379102E-2</v>
       </c>
     </row>
-    <row r="13" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D13" s="103">
         <v>0.8</v>
       </c>
@@ -7766,7 +8285,7 @@
         <v>-8.1811855697334597E-4</v>
       </c>
     </row>
-    <row r="14" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D14" s="103">
         <v>1</v>
       </c>
@@ -7809,7 +8328,7 @@
         <v>1.6852959410352447E-2</v>
       </c>
     </row>
-    <row r="15" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D15" s="58">
         <v>1.2</v>
       </c>
@@ -7850,7 +8369,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="16" spans="3:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:18" x14ac:dyDescent="0.3">
       <c r="D16" s="58">
         <v>1.4</v>
       </c>
@@ -7892,7 +8411,7 @@
       </c>
       <c r="R16" s="50"/>
     </row>
-    <row r="17" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D17" s="58">
         <v>1.6</v>
       </c>
@@ -7935,7 +8454,7 @@
         <v>0.69665730346768262</v>
       </c>
     </row>
-    <row r="18" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D18" s="58">
         <v>1.8</v>
       </c>
@@ -7952,7 +8471,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="19" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D19" s="58">
         <v>2</v>
       </c>
@@ -7969,7 +8488,7 @@
         <v>2320</v>
       </c>
     </row>
-    <row r="20" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D20" s="60">
         <v>2.4</v>
       </c>
@@ -7986,7 +8505,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="21" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D21" s="36"/>
       <c r="E21" s="36"/>
       <c r="F21" s="76">
@@ -7995,7 +8514,7 @@
       </c>
       <c r="G21" s="36"/>
     </row>
-    <row r="22" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:18" x14ac:dyDescent="0.3">
       <c r="D22" s="36"/>
       <c r="E22" s="36" t="s">
         <v>123</v>
@@ -8006,37 +8525,37 @@
       </c>
       <c r="G22" s="36"/>
     </row>
-    <row r="27" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:18" x14ac:dyDescent="0.3">
       <c r="R27" s="77" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:18" x14ac:dyDescent="0.3">
       <c r="R28" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="29" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:18" x14ac:dyDescent="0.3">
       <c r="R29" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="4:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:18" x14ac:dyDescent="0.3">
       <c r="R30" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="18:18" x14ac:dyDescent="0.3">
       <c r="R33" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="18:18" x14ac:dyDescent="0.3">
       <c r="R34" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="18:18" x14ac:dyDescent="0.3">
       <c r="R35" t="s">
         <v>119</v>
       </c>
@@ -8055,67 +8574,67 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:T38"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="X30" sqref="X30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="131" t="s">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="C3" s="130" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="132"/>
-      <c r="E3" s="132"/>
-      <c r="F3" s="132"/>
-      <c r="G3" s="132"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="132"/>
-      <c r="J3" s="132"/>
-      <c r="K3" s="133"/>
-      <c r="L3" s="131" t="s">
+      <c r="D3" s="131"/>
+      <c r="E3" s="131"/>
+      <c r="F3" s="131"/>
+      <c r="G3" s="131"/>
+      <c r="H3" s="131"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="131"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="130" t="s">
         <v>127</v>
       </c>
-      <c r="M3" s="132"/>
-      <c r="N3" s="132"/>
-      <c r="O3" s="132"/>
-      <c r="P3" s="132"/>
-      <c r="Q3" s="132"/>
-      <c r="R3" s="132"/>
-      <c r="S3" s="132"/>
-      <c r="T3" s="133"/>
-    </row>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C4" s="131" t="s">
+      <c r="M3" s="131"/>
+      <c r="N3" s="131"/>
+      <c r="O3" s="131"/>
+      <c r="P3" s="131"/>
+      <c r="Q3" s="131"/>
+      <c r="R3" s="131"/>
+      <c r="S3" s="131"/>
+      <c r="T3" s="132"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="C4" s="130" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
-      <c r="H4" s="132"/>
-      <c r="I4" s="132"/>
-      <c r="J4" s="132"/>
-      <c r="K4" s="133"/>
-      <c r="L4" s="134" t="s">
+      <c r="D4" s="131"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
+      <c r="H4" s="131"/>
+      <c r="I4" s="131"/>
+      <c r="J4" s="131"/>
+      <c r="K4" s="132"/>
+      <c r="L4" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="M4" s="134"/>
-      <c r="N4" s="134"/>
-      <c r="O4" s="134"/>
-      <c r="P4" s="134"/>
-      <c r="Q4" s="134"/>
-      <c r="R4" s="134"/>
-      <c r="S4" s="134"/>
-      <c r="T4" s="135"/>
-    </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="M4" s="133"/>
+      <c r="N4" s="133"/>
+      <c r="O4" s="133"/>
+      <c r="P4" s="133"/>
+      <c r="Q4" s="133"/>
+      <c r="R4" s="133"/>
+      <c r="S4" s="133"/>
+      <c r="T4" s="134"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B5" s="98" t="s">
         <v>124</v>
       </c>
@@ -8174,7 +8693,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B6" s="68">
         <v>35</v>
       </c>
@@ -8233,7 +8752,7 @@
         <v>5.7415540219392903E-6</v>
       </c>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B7" s="68">
         <f>B6+$C$12</f>
         <v>200</v>
@@ -8293,7 +8812,7 @@
         <v>-2.7105054312137601E-19</v>
       </c>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B8" s="68">
         <f>B7+$C$12</f>
         <v>365</v>
@@ -8353,7 +8872,7 @@
         <v>8.1370368257948704E-6</v>
       </c>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B9" s="68">
         <f>B8+$C$12</f>
         <v>530</v>
@@ -8413,7 +8932,7 @@
         <v>-4.4487537785892303E-6</v>
       </c>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B10" s="63">
         <f>B9+$C$12</f>
         <v>695</v>
@@ -8473,7 +8992,7 @@
         <v>-2.3954828038556201E-5</v>
       </c>
     </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>128</v>
       </c>
@@ -8484,80 +9003,80 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
       <c r="H22" s="95"/>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C28" s="136" t="s">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="C28" s="135" t="s">
         <v>129</v>
       </c>
-      <c r="D28" s="137"/>
-      <c r="E28" s="137"/>
-      <c r="F28" s="137"/>
-      <c r="G28" s="137"/>
-      <c r="H28" s="137"/>
-      <c r="I28" s="137"/>
-      <c r="J28" s="137"/>
-      <c r="K28" s="137"/>
-      <c r="L28" s="137"/>
-      <c r="M28" s="137"/>
-      <c r="N28" s="137"/>
-      <c r="O28" s="137"/>
-      <c r="P28" s="137"/>
-      <c r="Q28" s="137"/>
-      <c r="R28" s="137"/>
-      <c r="S28" s="137"/>
-      <c r="T28" s="138"/>
-    </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C29" s="131" t="s">
+      <c r="D28" s="136"/>
+      <c r="E28" s="136"/>
+      <c r="F28" s="136"/>
+      <c r="G28" s="136"/>
+      <c r="H28" s="136"/>
+      <c r="I28" s="136"/>
+      <c r="J28" s="136"/>
+      <c r="K28" s="136"/>
+      <c r="L28" s="136"/>
+      <c r="M28" s="136"/>
+      <c r="N28" s="136"/>
+      <c r="O28" s="136"/>
+      <c r="P28" s="136"/>
+      <c r="Q28" s="136"/>
+      <c r="R28" s="136"/>
+      <c r="S28" s="136"/>
+      <c r="T28" s="137"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="C29" s="130" t="s">
         <v>126</v>
       </c>
-      <c r="D29" s="132"/>
-      <c r="E29" s="132"/>
-      <c r="F29" s="132"/>
-      <c r="G29" s="132"/>
-      <c r="H29" s="132"/>
-      <c r="I29" s="132"/>
-      <c r="J29" s="132"/>
-      <c r="K29" s="133"/>
-      <c r="L29" s="131" t="s">
+      <c r="D29" s="131"/>
+      <c r="E29" s="131"/>
+      <c r="F29" s="131"/>
+      <c r="G29" s="131"/>
+      <c r="H29" s="131"/>
+      <c r="I29" s="131"/>
+      <c r="J29" s="131"/>
+      <c r="K29" s="132"/>
+      <c r="L29" s="130" t="s">
         <v>127</v>
       </c>
-      <c r="M29" s="132"/>
-      <c r="N29" s="132"/>
-      <c r="O29" s="132"/>
-      <c r="P29" s="132"/>
-      <c r="Q29" s="132"/>
-      <c r="R29" s="132"/>
-      <c r="S29" s="132"/>
-      <c r="T29" s="133"/>
-    </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C30" s="131" t="s">
+      <c r="M29" s="131"/>
+      <c r="N29" s="131"/>
+      <c r="O29" s="131"/>
+      <c r="P29" s="131"/>
+      <c r="Q29" s="131"/>
+      <c r="R29" s="131"/>
+      <c r="S29" s="131"/>
+      <c r="T29" s="132"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="C30" s="130" t="s">
         <v>125</v>
       </c>
-      <c r="D30" s="132"/>
-      <c r="E30" s="132"/>
-      <c r="F30" s="132"/>
-      <c r="G30" s="132"/>
-      <c r="H30" s="132"/>
-      <c r="I30" s="132"/>
-      <c r="J30" s="132"/>
-      <c r="K30" s="133"/>
-      <c r="L30" s="134" t="s">
+      <c r="D30" s="131"/>
+      <c r="E30" s="131"/>
+      <c r="F30" s="131"/>
+      <c r="G30" s="131"/>
+      <c r="H30" s="131"/>
+      <c r="I30" s="131"/>
+      <c r="J30" s="131"/>
+      <c r="K30" s="132"/>
+      <c r="L30" s="133" t="s">
         <v>125</v>
       </c>
-      <c r="M30" s="134"/>
-      <c r="N30" s="134"/>
-      <c r="O30" s="134"/>
-      <c r="P30" s="134"/>
-      <c r="Q30" s="134"/>
-      <c r="R30" s="134"/>
-      <c r="S30" s="134"/>
-      <c r="T30" s="135"/>
-    </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="M30" s="133"/>
+      <c r="N30" s="133"/>
+      <c r="O30" s="133"/>
+      <c r="P30" s="133"/>
+      <c r="Q30" s="133"/>
+      <c r="R30" s="133"/>
+      <c r="S30" s="133"/>
+      <c r="T30" s="134"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B31" s="98" t="s">
         <v>124</v>
       </c>
@@ -8616,7 +9135,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B32" s="85">
         <v>35</v>
       </c>
@@ -8675,7 +9194,7 @@
         <v>1.47976197266107E-3</v>
       </c>
     </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B33" s="87">
         <f>B32+$C$38</f>
         <v>200</v>
@@ -8735,7 +9254,7 @@
         <v>2.2906138899979E-3</v>
       </c>
     </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B34" s="87">
         <f>B33+$C$38</f>
         <v>365</v>
@@ -8795,7 +9314,7 @@
         <v>1.8004905036217401E-3</v>
       </c>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B35" s="87">
         <f>B34+$C$38</f>
         <v>530</v>
@@ -8855,7 +9374,7 @@
         <v>1.3450065590600499E-3</v>
       </c>
     </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B36" s="114">
         <f>B35+$C$38</f>
         <v>695</v>
@@ -8915,7 +9434,7 @@
         <v>6.4043042643396203E-4</v>
       </c>
     </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>128</v>
       </c>
@@ -8944,25 +9463,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="C3:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:H4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="116"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="146" t="s">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C3" s="115"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="138" t="s">
         <v>132</v>
       </c>
       <c r="F3" s="139"/>
@@ -8971,11 +9490,11 @@
       </c>
       <c r="H3" s="141"/>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C4" s="68" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="115" t="s">
+      <c r="D4" t="s">
         <v>90</v>
       </c>
       <c r="E4" s="68" t="s">
@@ -8991,11 +9510,11 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C5" s="68">
         <v>0.05</v>
       </c>
-      <c r="D5" s="115">
+      <c r="D5">
         <v>0.375</v>
       </c>
       <c r="E5" s="68">
@@ -9004,18 +9523,18 @@
       <c r="F5" s="69">
         <v>83</v>
       </c>
-      <c r="G5" s="142">
+      <c r="G5" s="68">
         <v>2257</v>
       </c>
-      <c r="H5" s="143">
+      <c r="H5" s="69">
         <v>3863</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C6" s="68">
         <v>0.1</v>
       </c>
-      <c r="D6" s="115">
+      <c r="D6">
         <v>0.75</v>
       </c>
       <c r="E6" s="68">
@@ -9024,18 +9543,18 @@
       <c r="F6" s="69">
         <v>146</v>
       </c>
-      <c r="G6" s="142">
+      <c r="G6" s="68">
         <v>3863</v>
       </c>
-      <c r="H6" s="143">
+      <c r="H6" s="69">
         <v>5667</v>
       </c>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C7" s="68">
         <v>0.15</v>
       </c>
-      <c r="D7" s="115">
+      <c r="D7">
         <v>1.125</v>
       </c>
       <c r="E7" s="68">
@@ -9044,18 +9563,18 @@
       <c r="F7" s="69">
         <v>329</v>
       </c>
-      <c r="G7" s="142">
+      <c r="G7" s="68">
         <v>5667</v>
       </c>
-      <c r="H7" s="143">
+      <c r="H7" s="69">
         <v>7421</v>
       </c>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C8" s="68">
         <v>0.2</v>
       </c>
-      <c r="D8" s="115">
+      <c r="D8">
         <v>1.5</v>
       </c>
       <c r="E8" s="68">
@@ -9064,18 +9583,18 @@
       <c r="F8" s="69">
         <v>452</v>
       </c>
-      <c r="G8" s="142">
+      <c r="G8" s="68">
         <v>7421</v>
       </c>
-      <c r="H8" s="143">
+      <c r="H8" s="69">
         <v>9091</v>
       </c>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C9" s="68">
         <v>0.3</v>
       </c>
-      <c r="D9" s="115">
+      <c r="D9">
         <v>2.25</v>
       </c>
       <c r="E9" s="68">
@@ -9084,18 +9603,18 @@
       <c r="F9" s="69">
         <v>635</v>
       </c>
-      <c r="G9" s="142">
+      <c r="G9" s="68">
         <v>9091</v>
       </c>
-      <c r="H9" s="143">
+      <c r="H9" s="69">
         <v>10847</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10" s="68">
         <v>0.4</v>
       </c>
-      <c r="D10" s="115">
+      <c r="D10">
         <v>3</v>
       </c>
       <c r="E10" s="68">
@@ -9104,18 +9623,18 @@
       <c r="F10" s="69">
         <v>878</v>
       </c>
-      <c r="G10" s="142">
+      <c r="G10" s="68">
         <v>10847</v>
       </c>
-      <c r="H10" s="143">
+      <c r="H10" s="69">
         <v>13190</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11" s="68">
         <v>0.6</v>
       </c>
-      <c r="D11" s="115">
+      <c r="D11">
         <v>4.5</v>
       </c>
       <c r="E11" s="68">
@@ -9124,18 +9643,18 @@
       <c r="F11" s="69">
         <v>1241</v>
       </c>
-      <c r="G11" s="142">
+      <c r="G11" s="68">
         <v>13190</v>
       </c>
-      <c r="H11" s="143">
+      <c r="H11" s="69">
         <v>15915</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C12" s="68">
         <v>0.8</v>
       </c>
-      <c r="D12" s="115">
+      <c r="D12">
         <v>6</v>
       </c>
       <c r="E12" s="68">
@@ -9144,18 +9663,18 @@
       <c r="F12" s="69">
         <v>1724</v>
       </c>
-      <c r="G12" s="142">
+      <c r="G12" s="68">
         <v>15915</v>
       </c>
-      <c r="H12" s="143">
+      <c r="H12" s="69">
         <v>18249</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C13" s="68">
         <v>1</v>
       </c>
-      <c r="D13" s="115">
+      <c r="D13">
         <v>7.5</v>
       </c>
       <c r="E13" s="68">
@@ -9164,18 +9683,18 @@
       <c r="F13" s="69">
         <v>2327</v>
       </c>
-      <c r="G13" s="142">
+      <c r="G13" s="68">
         <v>18249</v>
       </c>
-      <c r="H13" s="143">
+      <c r="H13" s="69">
         <v>20816</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C14" s="68">
         <v>1.2</v>
       </c>
-      <c r="D14" s="115">
+      <c r="D14">
         <v>9</v>
       </c>
       <c r="E14" s="68">
@@ -9184,18 +9703,18 @@
       <c r="F14" s="69">
         <v>3050</v>
       </c>
-      <c r="G14" s="142">
+      <c r="G14" s="68">
         <v>20816</v>
       </c>
-      <c r="H14" s="143">
+      <c r="H14" s="69">
         <v>23524</v>
       </c>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C15" s="68">
         <v>1.4</v>
       </c>
-      <c r="D15" s="115">
+      <c r="D15">
         <v>10.5</v>
       </c>
       <c r="E15" s="68">
@@ -9204,18 +9723,18 @@
       <c r="F15" s="69">
         <v>3893</v>
       </c>
-      <c r="G15" s="142">
+      <c r="G15" s="68">
         <v>23524</v>
       </c>
-      <c r="H15" s="143">
+      <c r="H15" s="69">
         <v>25768</v>
       </c>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C16" s="68">
         <v>1.6</v>
       </c>
-      <c r="D16" s="115">
+      <c r="D16">
         <v>12</v>
       </c>
       <c r="E16" s="68">
@@ -9224,18 +9743,18 @@
       <c r="F16" s="69">
         <v>4856</v>
       </c>
-      <c r="G16" s="142">
+      <c r="G16" s="68">
         <v>25768</v>
       </c>
-      <c r="H16" s="143">
+      <c r="H16" s="69">
         <v>27955</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C17" s="68">
         <v>1.8</v>
       </c>
-      <c r="D17" s="115">
+      <c r="D17">
         <v>13.5</v>
       </c>
       <c r="E17" s="68">
@@ -9244,18 +9763,18 @@
       <c r="F17" s="69">
         <v>5939</v>
       </c>
-      <c r="G17" s="142">
+      <c r="G17" s="68">
         <v>27955</v>
       </c>
-      <c r="H17" s="143">
+      <c r="H17" s="69">
         <v>29735</v>
       </c>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C18" s="68">
         <v>2</v>
       </c>
-      <c r="D18" s="115">
+      <c r="D18">
         <v>15</v>
       </c>
       <c r="E18" s="68">
@@ -9264,14 +9783,14 @@
       <c r="F18" s="69">
         <v>7142</v>
       </c>
-      <c r="G18" s="142">
+      <c r="G18" s="68">
         <v>29735</v>
       </c>
-      <c r="H18" s="143">
+      <c r="H18" s="69">
         <v>31407</v>
       </c>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C19" s="63">
         <v>2.4</v>
       </c>
@@ -9284,10 +9803,10 @@
       <c r="F19" s="97">
         <v>8585</v>
       </c>
-      <c r="G19" s="144">
+      <c r="G19" s="63">
         <v>31407</v>
       </c>
-      <c r="H19" s="145">
+      <c r="H19" s="97">
         <v>33198</v>
       </c>
     </row>

</xml_diff>